<commit_message>
Weekly report for all the batches
</commit_message>
<xml_diff>
--- a/18th_September_Batch_Java_Full_Stack/Weekly_Status_Report/JSpiders - HTD - Java Full Stack - Weekly Status Report for Capgemini - Detailed.xlsx
+++ b/18th_September_Batch_Java_Full_Stack/Weekly_Status_Report/JSpiders - HTD - Java Full Stack - Weekly Status Report for Capgemini - Detailed.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Week</t>
   </si>
@@ -59,12 +59,6 @@
     <t>18 Sep 2019 
 to 
 22 Sep 2019</t>
-  </si>
-  <si>
-    <t>18 Aug - 22 Aug</t>
-  </si>
-  <si>
-    <t>23 Aug - 29 Aug</t>
   </si>
   <si>
     <r>
@@ -146,9 +140,6 @@
 06 Oct 2019</t>
   </si>
   <si>
-    <t>Continuing Java, SQL and JDBC</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -176,6 +167,30 @@
 o How to Constrain the Result Set
 o DISTINCT and NOT DISTINCT</t>
     </r>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>18 Sep - 22 Sep</t>
+  </si>
+  <si>
+    <t>23 Sep - 29 Sep</t>
+  </si>
+  <si>
+    <t>Continuing Java and JDBC
+SQL Completed</t>
+  </si>
+  <si>
+    <t>30 Sep - 06 Oct</t>
+  </si>
+  <si>
+    <t>07 Oct 2019 
+to 
+13 Oct 2019</t>
+  </si>
+  <si>
+    <t>Completeing Java and JDBC</t>
   </si>
 </sst>
 </file>
@@ -452,41 +467,41 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,7 +526,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="314325"/>
@@ -554,7 +569,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="314325"/>
@@ -597,7 +612,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -640,7 +655,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -683,7 +698,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -726,7 +741,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -769,7 +784,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -812,7 +827,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -855,7 +870,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -898,7 +913,7 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="314325"/>
@@ -941,7 +956,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="314325"/>
@@ -984,7 +999,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -1027,7 +1042,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -1070,7 +1085,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -1113,7 +1128,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -1156,7 +1171,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -1199,7 +1214,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -1242,7 +1257,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304800" cy="304800"/>
@@ -1262,6 +1277,393 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="276225" y="21974175"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="314325"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="AutoShape 9" descr="Image result for covalense logo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D428B74-D5C9-774F-A649-26F771A05E1E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1114425" y="7343775"/>
+          <a:ext cx="304800" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="314325"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="AutoShape 11" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAfYAAABbCAMAAAC2wFcKAAAAY1BMVEX///8AjNHv+PwfmtcPk9R/xehvvuXP6fav2/EGj9L5/P6f1O4vodn7/f71+v0FjtIWltXh8frH5vWHyenA4/TX7fg8p9wrn9mTzuxTseBft+KW0OxHrN5zwOa43/Lo9fuo2O9Of94sAAARxUlEQVR4nO1d6ZqiOhBVRFwAxQ0FEXj/p7yyKKeSygKxb09/3fVrxoZQyUlqTzKbGcgrb0ERLfz5k/wkKvJbWZne+aMfTV6dX+cMXYP19rt5+wx5Q6cW383Lv0FeWOw5zDvy8+N3M/gJ+oOd0iX31Zh3FNXxd3PpTH+wI60yE+Yd8OV3M+pKf7APdLADvaHsh5t3f7C/aLvcWKM+nyfr7+bXif5g72kVjQC9oeVP1vB/sHd0H7PUO8p23830dPqDvaE4GA36k9Kfi/sf7E/acrbcJg3u5ergeV51OYePlHHmfy7uf7DPZrtCAnQRnMV43G6dSchnP1W//8E+iyXUi5KHs3qIFsDjf+b1U/QH+ywXRbcm/Cq59j80cPMH+43i6If6x0O64JOfGbf59bAfqcKODsYXEvJC9n8w+XH67bDvFhREi8TqiuL+I8X8b4edOuyB1TtHIuevP9Ga/+WwHwnqueVbIXmr/kL+vop+Oewp4ldYr1tiz//E5f67Ya8JfJ71exWpxfiBybhfDXuMFXP784g3iddXfBmDX0a/GvY1gmdnzvUUEwfA6PT9c/SrYUfN7tuL+IbuCPvpi/j7OvrNsK8coNui8x7xz8SrMCgi/+nu7f0kzZfluJk1nrzzLciiRfPF+eb5ySy4H/kkoR3s1XqZRUljx/hJlC3XYyOS8fGUpwt//3x/UQT3i/mNS/goomTffzG4Ha0L1O15RZ995GKfzZbwMmcM7mqmBjc6iV0v4a8WxkUMs60mf9mWAVvbP0+lb86sYL8s5faipQK6oavvoYjXmTgAi8dK17cyT+YibdKThQodw2uMXI3S7A0dXmw9uIl1eajqrlNabo04WoQNYJb4uBDO2jpvOaNogj2uVTVmKRuVlGDf3hYjXn9StZQx54fMkVdcaPPxmx7SuV+czqwMPYhJPULXGp99DH/wzRINGoaJujbWAUaCJDHAXvOCg2+rIRH2Ut1Ayi3C3VK7PeGqyY+N5RVl/AS7ZqVSVfHJVJdXwKtoYBgDADto+T1RL6n0AYZyooi0sBsbzCX5RmHfaWvUNrIZddRB1xI7WSbxilJotIxX08WiBHdzH56Hx43ZPAgvXV+/nTRbt5CuqCN1sIfGfUHzRFxEBPbKCIUgtGuL+lWfXRPjeT3g3z6XRivNjLQ9fwt0iPxsTHYl1AH1S4YtA+TpCvNeDbtdNen+Tt9C2A/GpStYMXfj8+0nZUE/hVfMp1hoVUu6Kb8uUPGyCiqY6oYSjwoWdofhCNSfgnJoSQn7zrbBJXkNYK/MqM/nN3h3bX68pb243ifximbXx8KrJ0tGnhS9cAfmDXzcpCe1tqNEw2CrYB8xjQjuA+xGCd+SP2ici514pC9N5zXif3YiO3HVU9GLGPAo9vqACLBcj//eU829lYgK9jHCA2XnAJ3lRBzMGKtp0hFdFZN4jdGM+FAOrZQ+t8jD86GptF8v5e71Gg5d95uu+cvwnN+KioOwUPZRW9pfdaX9QSQZe28bWgH7UnwhyW/lxfO8wzGUokGYu+JX7CIIj1Xz8l0OK7ws81p4JT/Vx6YHh0t5k+I9Z2deiUX3mTrISgw4ZMSIrE7i33tVDq67IswrdbSbMXS+X29iN6qb0P23+c/DLk7b/ExMbjEGtRi+x8FODoDY3oXwzcuqIxxmQvhEjMSAqzORV3wt0Q22PQlSp5BczZ3g0W86ZYWuuy5uDSN0Ft97esNcKCsO6VR7DSsLuyfUFcq8eNR0HgxyGXap94Iz38krCgMXnb6RIXtr96m8olrUrjFrohbp5s49Izj1vbKCHzVWBhSAdVDhNPNVYcaKfPEl5VnYyTjxfvLsSIb7jZMI+4bzSUKidLr2wRRY8MH3M7b91lJTeUXV8JGiZ1KzMU8UMAgbrzpewELXhAuhp+3k8GAdaGpEPOTrZRRxsK8QlasqAUKm0dslFGBX9J74OV2EDISRKk1TAl+vBTqZV5wuH9nSROoqE2WqibodXTcqLuYqElp+bT9RXulcESwTfWHMwY6MXdXWjodj+QpzUdg3qt6jWdvaGWBhqRNRYPu8rLDJvOKLWvvZlkiBliazsyUmfSn2QhkmBi3YTVxo56oNN6GA6Q0ABnbwE+aJLtlZgex8LXcKu3I8SaFyTDul9qY8X3xqOq84FobgmBWdrfrdsoJWVqdfMJ+qSjLC1Gj59fbCD0pCOdSvDAZ2FH/6WDWaYb0pRWDXmEqp8Cqwplkponpz4BUZqLVv2hGGKVL9o0QdtDigAFd0AzR5F7oHCzLRl2xXMkwy7FtAzmTrwJLp9SOBXQMEavcGZ1BUmtgJYFc48oqwfyBag5wojZMX4bc7wQDqS9EPmCudFoQZb7JNgLeeNRl2DJuY6lkAhkT6gjaJjTJxzfWKJW/fnP76uNXni+fIKyr7MaXSFv0xRvhL6WFwwRVpOJi13WraXY71bZk3pWemGhHoqxJ2kFZmx2YhNoiw68xL+G6rmdDpta90ceD1w7CjtWnO4oL5t+9QBnZYRQ2C2iDSGQLp0o+tBDuqGbPwA0nTedIIu3Y04TNNPzHilFiUWDrzioL2A9l2aM4ClpP0cTm5pnxjfN4ImOsxkWBHcWM+kUdUtgj7RutVCNObZEb8m92EduH1s7od2beohEQHpFsu4LqzaTgYLttFMZAF7DDtLGKWKHvaH3zb10FX3QTWGl64Kl+JXHhFB662+JaeLiNbA4XTayfwzxj3D9o3uAkcwZzpBZsEO6hLm32/IGbbSerbvi52U0odL4LalBhz4RUdLvdwDdqWNuk8DEV3v4AsYqYwmA5srF9N8fGBZkwv2CTY7dICb4JF2k4kgF2/zyQXHqy4MrooWOvKy1x4RY/fvcoCVK9VOg8L6Lpf0E6RJB1suTPW2wFV5bIQouUq2McfwvmidhrCV/ShI4C9G/WH3GJD+2h5Vml6F17RqnKvm4VJZCWE0YXrpQP0X5qG4B7apY28Y/gouA0KCtgr5lFLapkF2PX2sRRwq9Q1VX525ySnE68olt0zcKCyrI7EQFug96nAPpUCHrBG9KMaH8r7I4vUQ6mAfaV8wUhtf+GDem9Ygl0srxEoWkqxLydeMSvgnm8H/WGlMXbw9dc4gcoSIhcQAlR6h3Gza/BqlH8K2OVyMGtqPTg5DqggGXaVmB8YDOhwOPGKomJjg5SWADI7+1BKKhF9L2gdWBB8HHZ1Si3rTxWwh+o3TJQK3RkN+8xc7b5YQgzWjVfMgzmfSwBhN7t0HoxT3f8ERq2wpkGFMIO6u484Cl8B+8gSXCR32K3KzIt3u268fjReA9aTHezcC4Au0eCQfJPV0U4qzNSSAnbrXR0ytSy5wT472kzcrF+cbryiSnH24BiZrScOdshLECMTprekQUp+P7GSFLCP2NYh0idgn8WhxV6avmTOjVdM/kyIfDVe8RAQHr3aGSGPrjuJNQ9ySYzbbkdff/CPwt4caqC7fq+nkzuvxKabsgcunO/TZb/B3QX2QTw82Fag3kzI0jAH4cu0CHCz+eeF/Ad0e0/V3bhD5ubOK4qVKTm4zpnetNCPteRj9tvgkQLAMLtr0sjOOErXPGwifsCd2aS7euOonfcfgX3WIF9ofdB96cwrKvcpcToImKL7ZFWGi6IGvNIBHxDnw/QUNubqtpslaXA/elKzFg6cP2EoPgb7rLmlQ3EIT9cvz5VXdPsX4w8QJVWgoJasonSKjTAgv95CA75DJyfvvy7S/FSvaODeDDuOxZQLcD4Ie0OHMFP5J0tXXrfWJSEskeASKFkr8xAjksA6bGB/u2rwHRKtkoPZURDy55GZdTtOQ1MlIEcfhr1l6c5C7+9ceUUhaXu49JswYza/gv61EjywJ4dk7MB1v0jfuZImBCO+qNWpOTA4LVIxte0QAH0B7A2tTrJ5H7ryitJiM3bTK9nxthybbwd4SQQGWj1JTJJMNk1UR9r6Q9lt0CVep9g5XwR7w2koGK6ZK6/k4NixERvCzGVkdU2sqkaBtd1PBxBJJIRMvFf9pRe4PFSwQ3emJKa+DvaZGMO7uvJKtj/645Y7SQOlahx5QvVEq1FAk7dSHgwQ6rTjUBgOwkfjUwU7qowJGYovhV2IT3iOvNKjDcadME0mYDi2clZdXg0Top0PIPVJHAgLzjeGvmN8QwU7ugUTTk7+WtjpjT4XR14Fz3fMQZQkC5TsqOAwRuVRu+wF23uYTxHl0CcP4nYMk3jBXZ5195MEO66Aq7IlJU2DPa5WZXh6ZOnVN/g/ON5HR16FQo0Rt0fQQ2OaaYuC1LgrRpcOgKX5lPI7OAtI9ZhpmuE++JfIkHfFjIpZVpvkWmTBKSyPB4coHR7GoxeRiPTZkdeZcO6IdW1VTOy51iog5xaP2JwkiTpw3W9kgtDIAlp0htpycraPEnbUO0ZDCbVrO+kmCnnrWiwMZp8deZ3Rmjb74w2oy9ypF9QXkX7qkvCahNkwEwtsVaivw57rVfuFeHp98E+GnQQdDemkAzS5cYnJg6mm11RoylwceRXYmNtaGfRorEXXlv2dBJX+BoJhgW92IEME1pAH7ULZ0QoGJexEBPn6mYSGdSciJ8KOdeNaTwodp60jr23/aZlCYBGbFw5Eq/ufkRXddUP0NAt5swO47msw3ITOoZDXTdatkJvtJyQDO7FSI12wm2Q+O906EXYUttrlDrI0cuW1JeHE09Tkvu+EvNd7BpHCX9uzaxImzjLI73z4p2j54dcW6mCNlJHvpwgD+45EwAv1WJbkuKDut6kOHLNhh6MLfDJw5bUjAUbDjc4roepruNGZnlTlK9a7gAOXnB/UxWJoUuSK6BTlcpcPOe+jE9yRRbQ0MVX5NeTAsHnd/TgVdlyMyjPW6GFbZ1deO9qJQ8PdjvB69iFkBvYgN2j9tnj0dkcCDvyFkUw9obQFingOCrMmvslV1L0o5WDf0jT3gkfhzl5wOxV2kkb0Fc4YOWes+6ILrz1dpPxeumbh8OQiVWK7CadQyhcebIVTKBXHUDBVQ7Liox9bygzH7FUivU5ijyMU9x0E8iK6CErjtUImR+no3oiAU7FnYn7dnXl90VGu40ke4sa73TqXH6NomM6clW7NUQjnSq4llNeBYJNca6rgDye+RKX3HPgzZ8WCzM2DztyzWM/z7v9k2IWqAV+8OyouKXhvO2Y6r28qufotv3iEx+bE4upSho+UeyQTpsZZegJPmJbAVGZQpCOzmTB/LMLqZ7fycuiOZs6VZUl9dp+HXdJ3z+kUhMe2A+VJvq5riGtOj8lLou3aHBTdHpK9Wp+kM6bf8386r4DXpL2zcrpz1IYNdTBYuk+BiyNN2xPUpwAUB4tL8kpL/oDwdNjjEefJkyU7mVeg46g2OuKwGFHDrTwpVajcaYgNv9qP1wMWf2dOqK4RkO0cNaE565CBO4z4JHHRp/KKZHfXBRB7hvII3CNdgEDYBMrHnW3Hy1+j1uhMIuVdMSvrsdygn+2SeGVMKwUJK2Uir4Ri6TYCLUWq/Edo14lMW/MpbOFWnFtip5oahwL61pny6puhDpb7KGlgwinfbqtiJfk4jVeBrPbfdbRZqlFbWezm4g+bByKsKM8tsRgvv/2SdFCp5h44MQzJU0QhcCuzsFu2mTwMk3gVKQ4t9xFm2nakmI5E8r0SIhH7Vp0QPpoYzjtOsZqunfnaWx/N2yn3YpzAsbqmMl/34/MrZQKvMsWhxYrPjMXZYqCAkvJ2WyDiumuer7TTfdgTDpZLG57V3/FquHGVuaLDuahqrZeRezaQM41XllaBVuJcl1ZFeysmttOzYbcRA6a/vjbvrJpim4DfbtMWZ5ludN6JlwtBuzkD7Ad2vNZqozp56AZ9LK8qWp3EY716Sk/29XZeKDeyKaTLm1QE2thU/LF6yIIuydfE+sDCqkZaWtzfvnowo+ln/C6Mj5RQXk5ySKvpinQNuRuvOrqsT3kRLfx2uPwkylQbjTQUr25BcfWbIdk0W9P4W78V7w7bNC02YR/CRxElm57VR83ckyRsUYX/q5v1ymWeXv2+3eIRrlQAQHN6jHYCH+Kfz/fg2ZNmyPb+IsqXoe1Rq3a8/gfELfO2gTNXMAAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9750DD89-7F3E-894F-9D5A-D6FA80504B45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="7343775"/>
+          <a:ext cx="304800" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="AutoShape 12" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAfYAAABbCAMAAAC2wFcKAAAAY1BMVEX///8AjNHv+PwfmtcPk9R/xehvvuXP6fav2/EGj9L5/P6f1O4vodn7/f71+v0FjtIWltXh8frH5vWHyenA4/TX7fg8p9wrn9mTzuxTseBft+KW0OxHrN5zwOa43/Lo9fuo2O9Of94sAAARxUlEQVR4nO1d6ZqiOhBVRFwAxQ0FEXj/p7yyKKeSygKxb09/3fVrxoZQyUlqTzKbGcgrb0ERLfz5k/wkKvJbWZne+aMfTV6dX+cMXYP19rt5+wx5Q6cW383Lv0FeWOw5zDvy8+N3M/gJ+oOd0iX31Zh3FNXxd3PpTH+wI60yE+Yd8OV3M+pKf7APdLADvaHsh5t3f7C/aLvcWKM+nyfr7+bXif5g72kVjQC9oeVP1vB/sHd0H7PUO8p23830dPqDvaE4GA36k9Kfi/sf7E/acrbcJg3u5ergeV51OYePlHHmfy7uf7DPZrtCAnQRnMV43G6dSchnP1W//8E+iyXUi5KHs3qIFsDjf+b1U/QH+ywXRbcm/Cq59j80cPMH+43i6If6x0O64JOfGbf59bAfqcKODsYXEvJC9n8w+XH67bDvFhREi8TqiuL+I8X8b4edOuyB1TtHIuevP9Ga/+WwHwnqueVbIXmr/kL+vop+Oewp4ldYr1tiz//E5f67Ya8JfJ71exWpxfiBybhfDXuMFXP784g3iddXfBmDX0a/GvY1gmdnzvUUEwfA6PT9c/SrYUfN7tuL+IbuCPvpi/j7OvrNsK8coNui8x7xz8SrMCgi/+nu7f0kzZfluJk1nrzzLciiRfPF+eb5ySy4H/kkoR3s1XqZRUljx/hJlC3XYyOS8fGUpwt//3x/UQT3i/mNS/goomTffzG4Ha0L1O15RZ995GKfzZbwMmcM7mqmBjc6iV0v4a8WxkUMs60mf9mWAVvbP0+lb86sYL8s5faipQK6oavvoYjXmTgAi8dK17cyT+YibdKThQodw2uMXI3S7A0dXmw9uIl1eajqrlNabo04WoQNYJb4uBDO2jpvOaNogj2uVTVmKRuVlGDf3hYjXn9StZQx54fMkVdcaPPxmx7SuV+czqwMPYhJPULXGp99DH/wzRINGoaJujbWAUaCJDHAXvOCg2+rIRH2Ut1Ayi3C3VK7PeGqyY+N5RVl/AS7ZqVSVfHJVJdXwKtoYBgDADto+T1RL6n0AYZyooi0sBsbzCX5RmHfaWvUNrIZddRB1xI7WSbxilJotIxX08WiBHdzH56Hx43ZPAgvXV+/nTRbt5CuqCN1sIfGfUHzRFxEBPbKCIUgtGuL+lWfXRPjeT3g3z6XRivNjLQ9fwt0iPxsTHYl1AH1S4YtA+TpCvNeDbtdNen+Tt9C2A/GpStYMXfj8+0nZUE/hVfMp1hoVUu6Kb8uUPGyCiqY6oYSjwoWdofhCNSfgnJoSQn7zrbBJXkNYK/MqM/nN3h3bX68pb243ifximbXx8KrJ0tGnhS9cAfmDXzcpCe1tqNEw2CrYB8xjQjuA+xGCd+SP2ici514pC9N5zXif3YiO3HVU9GLGPAo9vqACLBcj//eU829lYgK9jHCA2XnAJ3lRBzMGKtp0hFdFZN4jdGM+FAOrZQ+t8jD86GptF8v5e71Gg5d95uu+cvwnN+KioOwUPZRW9pfdaX9QSQZe28bWgH7UnwhyW/lxfO8wzGUokGYu+JX7CIIj1Xz8l0OK7ws81p4JT/Vx6YHh0t5k+I9Z2deiUX3mTrISgw4ZMSIrE7i33tVDq67IswrdbSbMXS+X29iN6qb0P23+c/DLk7b/ExMbjEGtRi+x8FODoDY3oXwzcuqIxxmQvhEjMSAqzORV3wt0Q22PQlSp5BczZ3g0W86ZYWuuy5uDSN0Ft97esNcKCsO6VR7DSsLuyfUFcq8eNR0HgxyGXap94Iz38krCgMXnb6RIXtr96m8olrUrjFrohbp5s49Izj1vbKCHzVWBhSAdVDhNPNVYcaKfPEl5VnYyTjxfvLsSIb7jZMI+4bzSUKidLr2wRRY8MH3M7b91lJTeUXV8JGiZ1KzMU8UMAgbrzpewELXhAuhp+3k8GAdaGpEPOTrZRRxsK8QlasqAUKm0dslFGBX9J74OV2EDISRKk1TAl+vBTqZV5wuH9nSROoqE2WqibodXTcqLuYqElp+bT9RXulcESwTfWHMwY6MXdXWjodj+QpzUdg3qt6jWdvaGWBhqRNRYPu8rLDJvOKLWvvZlkiBliazsyUmfSn2QhkmBi3YTVxo56oNN6GA6Q0ABnbwE+aJLtlZgex8LXcKu3I8SaFyTDul9qY8X3xqOq84FobgmBWdrfrdsoJWVqdfMJ+qSjLC1Gj59fbCD0pCOdSvDAZ2FH/6WDWaYb0pRWDXmEqp8Cqwplkponpz4BUZqLVv2hGGKVL9o0QdtDigAFd0AzR5F7oHCzLRl2xXMkwy7FtAzmTrwJLp9SOBXQMEavcGZ1BUmtgJYFc48oqwfyBag5wojZMX4bc7wQDqS9EPmCudFoQZb7JNgLeeNRl2DJuY6lkAhkT6gjaJjTJxzfWKJW/fnP76uNXni+fIKyr7MaXSFv0xRvhL6WFwwRVpOJi13WraXY71bZk3pWemGhHoqxJ2kFZmx2YhNoiw68xL+G6rmdDpta90ceD1w7CjtWnO4oL5t+9QBnZYRQ2C2iDSGQLp0o+tBDuqGbPwA0nTedIIu3Y04TNNPzHilFiUWDrzioL2A9l2aM4ClpP0cTm5pnxjfN4ImOsxkWBHcWM+kUdUtgj7RutVCNObZEb8m92EduH1s7od2beohEQHpFsu4LqzaTgYLttFMZAF7DDtLGKWKHvaH3zb10FX3QTWGl64Kl+JXHhFB662+JaeLiNbA4XTayfwzxj3D9o3uAkcwZzpBZsEO6hLm32/IGbbSerbvi52U0odL4LalBhz4RUdLvdwDdqWNuk8DEV3v4AsYqYwmA5srF9N8fGBZkwv2CTY7dICb4JF2k4kgF2/zyQXHqy4MrooWOvKy1x4RY/fvcoCVK9VOg8L6Lpf0E6RJB1suTPW2wFV5bIQouUq2McfwvmidhrCV/ShI4C9G/WH3GJD+2h5Vml6F17RqnKvm4VJZCWE0YXrpQP0X5qG4B7apY28Y/gouA0KCtgr5lFLapkF2PX2sRRwq9Q1VX525ySnE68olt0zcKCyrI7EQFug96nAPpUCHrBG9KMaH8r7I4vUQ6mAfaV8wUhtf+GDem9Ygl0srxEoWkqxLydeMSvgnm8H/WGlMXbw9dc4gcoSIhcQAlR6h3Gza/BqlH8K2OVyMGtqPTg5DqggGXaVmB8YDOhwOPGKomJjg5SWADI7+1BKKhF9L2gdWBB8HHZ1Si3rTxWwh+o3TJQK3RkN+8xc7b5YQgzWjVfMgzmfSwBhN7t0HoxT3f8ERq2wpkGFMIO6u484Cl8B+8gSXCR32K3KzIt3u268fjReA9aTHezcC4Au0eCQfJPV0U4qzNSSAnbrXR0ytSy5wT472kzcrF+cbryiSnH24BiZrScOdshLECMTprekQUp+P7GSFLCP2NYh0idgn8WhxV6avmTOjVdM/kyIfDVe8RAQHr3aGSGPrjuJNQ9ySYzbbkdff/CPwt4caqC7fq+nkzuvxKabsgcunO/TZb/B3QX2QTw82Fag3kzI0jAH4cu0CHCz+eeF/Ad0e0/V3bhD5ubOK4qVKTm4zpnetNCPteRj9tvgkQLAMLtr0sjOOErXPGwifsCd2aS7euOonfcfgX3WIF9ofdB96cwrKvcpcToImKL7ZFWGi6IGvNIBHxDnw/QUNubqtpslaXA/elKzFg6cP2EoPgb7rLmlQ3EIT9cvz5VXdPsX4w8QJVWgoJasonSKjTAgv95CA75DJyfvvy7S/FSvaODeDDuOxZQLcD4Ie0OHMFP5J0tXXrfWJSEskeASKFkr8xAjksA6bGB/u2rwHRKtkoPZURDy55GZdTtOQ1MlIEcfhr1l6c5C7+9ceUUhaXu49JswYza/gv61EjywJ4dk7MB1v0jfuZImBCO+qNWpOTA4LVIxte0QAH0B7A2tTrJ5H7ryitJiM3bTK9nxthybbwd4SQQGWj1JTJJMNk1UR9r6Q9lt0CVep9g5XwR7w2koGK6ZK6/k4NixERvCzGVkdU2sqkaBtd1PBxBJJIRMvFf9pRe4PFSwQ3emJKa+DvaZGMO7uvJKtj/645Y7SQOlahx5QvVEq1FAk7dSHgwQ6rTjUBgOwkfjUwU7qowJGYovhV2IT3iOvNKjDcadME0mYDi2clZdXg0Top0PIPVJHAgLzjeGvmN8QwU7ugUTTk7+WtjpjT4XR14Fz3fMQZQkC5TsqOAwRuVRu+wF23uYTxHl0CcP4nYMk3jBXZ5195MEO66Aq7IlJU2DPa5WZXh6ZOnVN/g/ON5HR16FQo0Rt0fQQ2OaaYuC1LgrRpcOgKX5lPI7OAtI9ZhpmuE++JfIkHfFjIpZVpvkWmTBKSyPB4coHR7GoxeRiPTZkdeZcO6IdW1VTOy51iog5xaP2JwkiTpw3W9kgtDIAlp0htpycraPEnbUO0ZDCbVrO+kmCnnrWiwMZp8deZ3Rmjb74w2oy9ypF9QXkX7qkvCahNkwEwtsVaivw57rVfuFeHp98E+GnQQdDemkAzS5cYnJg6mm11RoylwceRXYmNtaGfRorEXXlv2dBJX+BoJhgW92IEME1pAH7ULZ0QoGJexEBPn6mYSGdSciJ8KOdeNaTwodp60jr23/aZlCYBGbFw5Eq/ufkRXddUP0NAt5swO47msw3ITOoZDXTdatkJvtJyQDO7FSI12wm2Q+O906EXYUttrlDrI0cuW1JeHE09Tkvu+EvNd7BpHCX9uzaxImzjLI73z4p2j54dcW6mCNlJHvpwgD+45EwAv1WJbkuKDut6kOHLNhh6MLfDJw5bUjAUbDjc4roepruNGZnlTlK9a7gAOXnB/UxWJoUuSK6BTlcpcPOe+jE9yRRbQ0MVX5NeTAsHnd/TgVdlyMyjPW6GFbZ1deO9qJQ8PdjvB69iFkBvYgN2j9tnj0dkcCDvyFkUw9obQFingOCrMmvslV1L0o5WDf0jT3gkfhzl5wOxV2kkb0Fc4YOWes+6ILrz1dpPxeumbh8OQiVWK7CadQyhcebIVTKBXHUDBVQ7Liox9bygzH7FUivU5ijyMU9x0E8iK6CErjtUImR+no3oiAU7FnYn7dnXl90VGu40ke4sa73TqXH6NomM6clW7NUQjnSq4llNeBYJNca6rgDye+RKX3HPgzZ8WCzM2DztyzWM/z7v9k2IWqAV+8OyouKXhvO2Y6r28qufotv3iEx+bE4upSho+UeyQTpsZZegJPmJbAVGZQpCOzmTB/LMLqZ7fycuiOZs6VZUl9dp+HXdJ3z+kUhMe2A+VJvq5riGtOj8lLou3aHBTdHpK9Wp+kM6bf8386r4DXpL2zcrpz1IYNdTBYuk+BiyNN2xPUpwAUB4tL8kpL/oDwdNjjEefJkyU7mVeg46g2OuKwGFHDrTwpVajcaYgNv9qP1wMWf2dOqK4RkO0cNaE565CBO4z4JHHRp/KKZHfXBRB7hvII3CNdgEDYBMrHnW3Hy1+j1uhMIuVdMSvrsdygn+2SeGVMKwUJK2Uir4Ri6TYCLUWq/Edo14lMW/MpbOFWnFtip5oahwL61pny6puhDpb7KGlgwinfbqtiJfk4jVeBrPbfdbRZqlFbWezm4g+bByKsKM8tsRgvv/2SdFCp5h44MQzJU0QhcCuzsFu2mTwMk3gVKQ4t9xFm2nakmI5E8r0SIhH7Vp0QPpoYzjtOsZqunfnaWx/N2yn3YpzAsbqmMl/34/MrZQKvMsWhxYrPjMXZYqCAkvJ2WyDiumuer7TTfdgTDpZLG57V3/FquHGVuaLDuahqrZeRezaQM41XllaBVuJcl1ZFeysmttOzYbcRA6a/vjbvrJpim4DfbtMWZ5ludN6JlwtBuzkD7Ad2vNZqozp56AZ9LK8qWp3EY716Sk/29XZeKDeyKaTLm1QE2thU/LF6yIIuydfE+sDCqkZaWtzfvnowo+ln/C6Mj5RQXk5ySKvpinQNuRuvOrqsT3kRLfx2uPwkylQbjTQUr25BcfWbIdk0W9P4W78V7w7bNC02YR/CRxElm57VR83ckyRsUYX/q5v1ymWeXv2+3eIRrlQAQHN6jHYCH+Kfz/fg2ZNmyPb+IsqXoe1Rq3a8/gfELfO2gTNXMAAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9E8BECA-EF93-5D48-B7D2-6C8626A5163B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="7343775"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="AutoShape 11" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAfYAAABbCAMAAAC2wFcKAAAAY1BMVEX///8AjNHv+PwfmtcPk9R/xehvvuXP6fav2/EGj9L5/P6f1O4vodn7/f71+v0FjtIWltXh8frH5vWHyenA4/TX7fg8p9wrn9mTzuxTseBft+KW0OxHrN5zwOa43/Lo9fuo2O9Of94sAAARxUlEQVR4nO1d6ZqiOhBVRFwAxQ0FEXj/p7yyKKeSygKxb09/3fVrxoZQyUlqTzKbGcgrb0ERLfz5k/wkKvJbWZne+aMfTV6dX+cMXYP19rt5+wx5Q6cW383Lv0FeWOw5zDvy8+N3M/gJ+oOd0iX31Zh3FNXxd3PpTH+wI60yE+Yd8OV3M+pKf7APdLADvaHsh5t3f7C/aLvcWKM+nyfr7+bXif5g72kVjQC9oeVP1vB/sHd0H7PUO8p23830dPqDvaE4GA36k9Kfi/sf7E/acrbcJg3u5ergeV51OYePlHHmfy7uf7DPZrtCAnQRnMV43G6dSchnP1W//8E+iyXUi5KHs3qIFsDjf+b1U/QH+ywXRbcm/Cq59j80cPMH+43i6If6x0O64JOfGbf59bAfqcKODsYXEvJC9n8w+XH67bDvFhREi8TqiuL+I8X8b4edOuyB1TtHIuevP9Ga/+WwHwnqueVbIXmr/kL+vop+Oewp4ldYr1tiz//E5f67Ya8JfJ71exWpxfiBybhfDXuMFXP784g3iddXfBmDX0a/GvY1gmdnzvUUEwfA6PT9c/SrYUfN7tuL+IbuCPvpi/j7OvrNsK8coNui8x7xz8SrMCgi/+nu7f0kzZfluJk1nrzzLciiRfPF+eb5ySy4H/kkoR3s1XqZRUljx/hJlC3XYyOS8fGUpwt//3x/UQT3i/mNS/goomTffzG4Ha0L1O15RZ995GKfzZbwMmcM7mqmBjc6iV0v4a8WxkUMs60mf9mWAVvbP0+lb86sYL8s5faipQK6oavvoYjXmTgAi8dK17cyT+YibdKThQodw2uMXI3S7A0dXmw9uIl1eajqrlNabo04WoQNYJb4uBDO2jpvOaNogj2uVTVmKRuVlGDf3hYjXn9StZQx54fMkVdcaPPxmx7SuV+czqwMPYhJPULXGp99DH/wzRINGoaJujbWAUaCJDHAXvOCg2+rIRH2Ut1Ayi3C3VK7PeGqyY+N5RVl/AS7ZqVSVfHJVJdXwKtoYBgDADto+T1RL6n0AYZyooi0sBsbzCX5RmHfaWvUNrIZddRB1xI7WSbxilJotIxX08WiBHdzH56Hx43ZPAgvXV+/nTRbt5CuqCN1sIfGfUHzRFxEBPbKCIUgtGuL+lWfXRPjeT3g3z6XRivNjLQ9fwt0iPxsTHYl1AH1S4YtA+TpCvNeDbtdNen+Tt9C2A/GpStYMXfj8+0nZUE/hVfMp1hoVUu6Kb8uUPGyCiqY6oYSjwoWdofhCNSfgnJoSQn7zrbBJXkNYK/MqM/nN3h3bX68pb243ifximbXx8KrJ0tGnhS9cAfmDXzcpCe1tqNEw2CrYB8xjQjuA+xGCd+SP2ici514pC9N5zXif3YiO3HVU9GLGPAo9vqACLBcj//eU829lYgK9jHCA2XnAJ3lRBzMGKtp0hFdFZN4jdGM+FAOrZQ+t8jD86GptF8v5e71Gg5d95uu+cvwnN+KioOwUPZRW9pfdaX9QSQZe28bWgH7UnwhyW/lxfO8wzGUokGYu+JX7CIIj1Xz8l0OK7ws81p4JT/Vx6YHh0t5k+I9Z2deiUX3mTrISgw4ZMSIrE7i33tVDq67IswrdbSbMXS+X29iN6qb0P23+c/DLk7b/ExMbjEGtRi+x8FODoDY3oXwzcuqIxxmQvhEjMSAqzORV3wt0Q22PQlSp5BczZ3g0W86ZYWuuy5uDSN0Ft97esNcKCsO6VR7DSsLuyfUFcq8eNR0HgxyGXap94Iz38krCgMXnb6RIXtr96m8olrUrjFrohbp5s49Izj1vbKCHzVWBhSAdVDhNPNVYcaKfPEl5VnYyTjxfvLsSIb7jZMI+4bzSUKidLr2wRRY8MH3M7b91lJTeUXV8JGiZ1KzMU8UMAgbrzpewELXhAuhp+3k8GAdaGpEPOTrZRRxsK8QlasqAUKm0dslFGBX9J74OV2EDISRKk1TAl+vBTqZV5wuH9nSROoqE2WqibodXTcqLuYqElp+bT9RXulcESwTfWHMwY6MXdXWjodj+QpzUdg3qt6jWdvaGWBhqRNRYPu8rLDJvOKLWvvZlkiBliazsyUmfSn2QhkmBi3YTVxo56oNN6GA6Q0ABnbwE+aJLtlZgex8LXcKu3I8SaFyTDul9qY8X3xqOq84FobgmBWdrfrdsoJWVqdfMJ+qSjLC1Gj59fbCD0pCOdSvDAZ2FH/6WDWaYb0pRWDXmEqp8Cqwplkponpz4BUZqLVv2hGGKVL9o0QdtDigAFd0AzR5F7oHCzLRl2xXMkwy7FtAzmTrwJLp9SOBXQMEavcGZ1BUmtgJYFc48oqwfyBag5wojZMX4bc7wQDqS9EPmCudFoQZb7JNgLeeNRl2DJuY6lkAhkT6gjaJjTJxzfWKJW/fnP76uNXni+fIKyr7MaXSFv0xRvhL6WFwwRVpOJi13WraXY71bZk3pWemGhHoqxJ2kFZmx2YhNoiw68xL+G6rmdDpta90ceD1w7CjtWnO4oL5t+9QBnZYRQ2C2iDSGQLp0o+tBDuqGbPwA0nTedIIu3Y04TNNPzHilFiUWDrzioL2A9l2aM4ClpP0cTm5pnxjfN4ImOsxkWBHcWM+kUdUtgj7RutVCNObZEb8m92EduH1s7od2beohEQHpFsu4LqzaTgYLttFMZAF7DDtLGKWKHvaH3zb10FX3QTWGl64Kl+JXHhFB662+JaeLiNbA4XTayfwzxj3D9o3uAkcwZzpBZsEO6hLm32/IGbbSerbvi52U0odL4LalBhz4RUdLvdwDdqWNuk8DEV3v4AsYqYwmA5srF9N8fGBZkwv2CTY7dICb4JF2k4kgF2/zyQXHqy4MrooWOvKy1x4RY/fvcoCVK9VOg8L6Lpf0E6RJB1suTPW2wFV5bIQouUq2McfwvmidhrCV/ShI4C9G/WH3GJD+2h5Vml6F17RqnKvm4VJZCWE0YXrpQP0X5qG4B7apY28Y/gouA0KCtgr5lFLapkF2PX2sRRwq9Q1VX525ySnE68olt0zcKCyrI7EQFug96nAPpUCHrBG9KMaH8r7I4vUQ6mAfaV8wUhtf+GDem9Ygl0srxEoWkqxLydeMSvgnm8H/WGlMXbw9dc4gcoSIhcQAlR6h3Gza/BqlH8K2OVyMGtqPTg5DqggGXaVmB8YDOhwOPGKomJjg5SWADI7+1BKKhF9L2gdWBB8HHZ1Si3rTxWwh+o3TJQK3RkN+8xc7b5YQgzWjVfMgzmfSwBhN7t0HoxT3f8ERq2wpkGFMIO6u484Cl8B+8gSXCR32K3KzIt3u268fjReA9aTHezcC4Au0eCQfJPV0U4qzNSSAnbrXR0ytSy5wT472kzcrF+cbryiSnH24BiZrScOdshLECMTprekQUp+P7GSFLCP2NYh0idgn8WhxV6avmTOjVdM/kyIfDVe8RAQHr3aGSGPrjuJNQ9ySYzbbkdff/CPwt4caqC7fq+nkzuvxKabsgcunO/TZb/B3QX2QTw82Fag3kzI0jAH4cu0CHCz+eeF/Ad0e0/V3bhD5ubOK4qVKTm4zpnetNCPteRj9tvgkQLAMLtr0sjOOErXPGwifsCd2aS7euOonfcfgX3WIF9ofdB96cwrKvcpcToImKL7ZFWGi6IGvNIBHxDnw/QUNubqtpslaXA/elKzFg6cP2EoPgb7rLmlQ3EIT9cvz5VXdPsX4w8QJVWgoJasonSKjTAgv95CA75DJyfvvy7S/FSvaODeDDuOxZQLcD4Ie0OHMFP5J0tXXrfWJSEskeASKFkr8xAjksA6bGB/u2rwHRKtkoPZURDy55GZdTtOQ1MlIEcfhr1l6c5C7+9ceUUhaXu49JswYza/gv61EjywJ4dk7MB1v0jfuZImBCO+qNWpOTA4LVIxte0QAH0B7A2tTrJ5H7ryitJiM3bTK9nxthybbwd4SQQGWj1JTJJMNk1UR9r6Q9lt0CVep9g5XwR7w2koGK6ZK6/k4NixERvCzGVkdU2sqkaBtd1PBxBJJIRMvFf9pRe4PFSwQ3emJKa+DvaZGMO7uvJKtj/645Y7SQOlahx5QvVEq1FAk7dSHgwQ6rTjUBgOwkfjUwU7qowJGYovhV2IT3iOvNKjDcadME0mYDi2clZdXg0Top0PIPVJHAgLzjeGvmN8QwU7ugUTTk7+WtjpjT4XR14Fz3fMQZQkC5TsqOAwRuVRu+wF23uYTxHl0CcP4nYMk3jBXZ5195MEO66Aq7IlJU2DPa5WZXh6ZOnVN/g/ON5HR16FQo0Rt0fQQ2OaaYuC1LgrRpcOgKX5lPI7OAtI9ZhpmuE++JfIkHfFjIpZVpvkWmTBKSyPB4coHR7GoxeRiPTZkdeZcO6IdW1VTOy51iog5xaP2JwkiTpw3W9kgtDIAlp0htpycraPEnbUO0ZDCbVrO+kmCnnrWiwMZp8deZ3Rmjb74w2oy9ypF9QXkX7qkvCahNkwEwtsVaivw57rVfuFeHp98E+GnQQdDemkAzS5cYnJg6mm11RoylwceRXYmNtaGfRorEXXlv2dBJX+BoJhgW92IEME1pAH7ULZ0QoGJexEBPn6mYSGdSciJ8KOdeNaTwodp60jr23/aZlCYBGbFw5Eq/ufkRXddUP0NAt5swO47msw3ITOoZDXTdatkJvtJyQDO7FSI12wm2Q+O906EXYUttrlDrI0cuW1JeHE09Tkvu+EvNd7BpHCX9uzaxImzjLI73z4p2j54dcW6mCNlJHvpwgD+45EwAv1WJbkuKDut6kOHLNhh6MLfDJw5bUjAUbDjc4roepruNGZnlTlK9a7gAOXnB/UxWJoUuSK6BTlcpcPOe+jE9yRRbQ0MVX5NeTAsHnd/TgVdlyMyjPW6GFbZ1deO9qJQ8PdjvB69iFkBvYgN2j9tnj0dkcCDvyFkUw9obQFingOCrMmvslV1L0o5WDf0jT3gkfhzl5wOxV2kkb0Fc4YOWes+6ILrz1dpPxeumbh8OQiVWK7CadQyhcebIVTKBXHUDBVQ7Liox9bygzH7FUivU5ijyMU9x0E8iK6CErjtUImR+no3oiAU7FnYn7dnXl90VGu40ke4sa73TqXH6NomM6clW7NUQjnSq4llNeBYJNca6rgDye+RKX3HPgzZ8WCzM2DztyzWM/z7v9k2IWqAV+8OyouKXhvO2Y6r28qufotv3iEx+bE4upSho+UeyQTpsZZegJPmJbAVGZQpCOzmTB/LMLqZ7fycuiOZs6VZUl9dp+HXdJ3z+kUhMe2A+VJvq5riGtOj8lLou3aHBTdHpK9Wp+kM6bf8386r4DXpL2zcrpz1IYNdTBYuk+BiyNN2xPUpwAUB4tL8kpL/oDwdNjjEefJkyU7mVeg46g2OuKwGFHDrTwpVajcaYgNv9qP1wMWf2dOqK4RkO0cNaE565CBO4z4JHHRp/KKZHfXBRB7hvII3CNdgEDYBMrHnW3Hy1+j1uhMIuVdMSvrsdygn+2SeGVMKwUJK2Uir4Ri6TYCLUWq/Edo14lMW/MpbOFWnFtip5oahwL61pny6puhDpb7KGlgwinfbqtiJfk4jVeBrPbfdbRZqlFbWezm4g+bByKsKM8tsRgvv/2SdFCp5h44MQzJU0QhcCuzsFu2mTwMk3gVKQ4t9xFm2nakmI5E8r0SIhH7Vp0QPpoYzjtOsZqunfnaWx/N2yn3YpzAsbqmMl/34/MrZQKvMsWhxYrPjMXZYqCAkvJ2WyDiumuer7TTfdgTDpZLG57V3/FquHGVuaLDuahqrZeRezaQM41XllaBVuJcl1ZFeysmttOzYbcRA6a/vjbvrJpim4DfbtMWZ5ludN6JlwtBuzkD7Ad2vNZqozp56AZ9LK8qWp3EY716Sk/29XZeKDeyKaTLm1QE2thU/LF6yIIuydfE+sDCqkZaWtzfvnowo+ln/C6Mj5RQXk5ySKvpinQNuRuvOrqsT3kRLfx2uPwkylQbjTQUr25BcfWbIdk0W9P4W78V7w7bNC02YR/CRxElm57VR83ckyRsUYX/q5v1ymWeXv2+3eIRrlQAQHN6jHYCH+Kfz/fg2ZNmyPb+IsqXoe1Rq3a8/gfELfO2gTNXMAAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64609DCB-07D3-6148-9787-02BD5EF01DEB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="7343775"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="AutoShape 12" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAfYAAABbCAMAAAC2wFcKAAAAY1BMVEX///8AjNHv+PwfmtcPk9R/xehvvuXP6fav2/EGj9L5/P6f1O4vodn7/f71+v0FjtIWltXh8frH5vWHyenA4/TX7fg8p9wrn9mTzuxTseBft+KW0OxHrN5zwOa43/Lo9fuo2O9Of94sAAARxUlEQVR4nO1d6ZqiOhBVRFwAxQ0FEXj/p7yyKKeSygKxb09/3fVrxoZQyUlqTzKbGcgrb0ERLfz5k/wkKvJbWZne+aMfTV6dX+cMXYP19rt5+wx5Q6cW383Lv0FeWOw5zDvy8+N3M/gJ+oOd0iX31Zh3FNXxd3PpTH+wI60yE+Yd8OV3M+pKf7APdLADvaHsh5t3f7C/aLvcWKM+nyfr7+bXif5g72kVjQC9oeVP1vB/sHd0H7PUO8p23830dPqDvaE4GA36k9Kfi/sf7E/acrbcJg3u5ergeV51OYePlHHmfy7uf7DPZrtCAnQRnMV43G6dSchnP1W//8E+iyXUi5KHs3qIFsDjf+b1U/QH+ywXRbcm/Cq59j80cPMH+43i6If6x0O64JOfGbf59bAfqcKODsYXEvJC9n8w+XH67bDvFhREi8TqiuL+I8X8b4edOuyB1TtHIuevP9Ga/+WwHwnqueVbIXmr/kL+vop+Oewp4ldYr1tiz//E5f67Ya8JfJ71exWpxfiBybhfDXuMFXP784g3iddXfBmDX0a/GvY1gmdnzvUUEwfA6PT9c/SrYUfN7tuL+IbuCPvpi/j7OvrNsK8coNui8x7xz8SrMCgi/+nu7f0kzZfluJk1nrzzLciiRfPF+eb5ySy4H/kkoR3s1XqZRUljx/hJlC3XYyOS8fGUpwt//3x/UQT3i/mNS/goomTffzG4Ha0L1O15RZ995GKfzZbwMmcM7mqmBjc6iV0v4a8WxkUMs60mf9mWAVvbP0+lb86sYL8s5faipQK6oavvoYjXmTgAi8dK17cyT+YibdKThQodw2uMXI3S7A0dXmw9uIl1eajqrlNabo04WoQNYJb4uBDO2jpvOaNogj2uVTVmKRuVlGDf3hYjXn9StZQx54fMkVdcaPPxmx7SuV+czqwMPYhJPULXGp99DH/wzRINGoaJujbWAUaCJDHAXvOCg2+rIRH2Ut1Ayi3C3VK7PeGqyY+N5RVl/AS7ZqVSVfHJVJdXwKtoYBgDADto+T1RL6n0AYZyooi0sBsbzCX5RmHfaWvUNrIZddRB1xI7WSbxilJotIxX08WiBHdzH56Hx43ZPAgvXV+/nTRbt5CuqCN1sIfGfUHzRFxEBPbKCIUgtGuL+lWfXRPjeT3g3z6XRivNjLQ9fwt0iPxsTHYl1AH1S4YtA+TpCvNeDbtdNen+Tt9C2A/GpStYMXfj8+0nZUE/hVfMp1hoVUu6Kb8uUPGyCiqY6oYSjwoWdofhCNSfgnJoSQn7zrbBJXkNYK/MqM/nN3h3bX68pb243ifximbXx8KrJ0tGnhS9cAfmDXzcpCe1tqNEw2CrYB8xjQjuA+xGCd+SP2ici514pC9N5zXif3YiO3HVU9GLGPAo9vqACLBcj//eU829lYgK9jHCA2XnAJ3lRBzMGKtp0hFdFZN4jdGM+FAOrZQ+t8jD86GptF8v5e71Gg5d95uu+cvwnN+KioOwUPZRW9pfdaX9QSQZe28bWgH7UnwhyW/lxfO8wzGUokGYu+JX7CIIj1Xz8l0OK7ws81p4JT/Vx6YHh0t5k+I9Z2deiUX3mTrISgw4ZMSIrE7i33tVDq67IswrdbSbMXS+X29iN6qb0P23+c/DLk7b/ExMbjEGtRi+x8FODoDY3oXwzcuqIxxmQvhEjMSAqzORV3wt0Q22PQlSp5BczZ3g0W86ZYWuuy5uDSN0Ft97esNcKCsO6VR7DSsLuyfUFcq8eNR0HgxyGXap94Iz38krCgMXnb6RIXtr96m8olrUrjFrohbp5s49Izj1vbKCHzVWBhSAdVDhNPNVYcaKfPEl5VnYyTjxfvLsSIb7jZMI+4bzSUKidLr2wRRY8MH3M7b91lJTeUXV8JGiZ1KzMU8UMAgbrzpewELXhAuhp+3k8GAdaGpEPOTrZRRxsK8QlasqAUKm0dslFGBX9J74OV2EDISRKk1TAl+vBTqZV5wuH9nSROoqE2WqibodXTcqLuYqElp+bT9RXulcESwTfWHMwY6MXdXWjodj+QpzUdg3qt6jWdvaGWBhqRNRYPu8rLDJvOKLWvvZlkiBliazsyUmfSn2QhkmBi3YTVxo56oNN6GA6Q0ABnbwE+aJLtlZgex8LXcKu3I8SaFyTDul9qY8X3xqOq84FobgmBWdrfrdsoJWVqdfMJ+qSjLC1Gj59fbCD0pCOdSvDAZ2FH/6WDWaYb0pRWDXmEqp8Cqwplkponpz4BUZqLVv2hGGKVL9o0QdtDigAFd0AzR5F7oHCzLRl2xXMkwy7FtAzmTrwJLp9SOBXQMEavcGZ1BUmtgJYFc48oqwfyBag5wojZMX4bc7wQDqS9EPmCudFoQZb7JNgLeeNRl2DJuY6lkAhkT6gjaJjTJxzfWKJW/fnP76uNXni+fIKyr7MaXSFv0xRvhL6WFwwRVpOJi13WraXY71bZk3pWemGhHoqxJ2kFZmx2YhNoiw68xL+G6rmdDpta90ceD1w7CjtWnO4oL5t+9QBnZYRQ2C2iDSGQLp0o+tBDuqGbPwA0nTedIIu3Y04TNNPzHilFiUWDrzioL2A9l2aM4ClpP0cTm5pnxjfN4ImOsxkWBHcWM+kUdUtgj7RutVCNObZEb8m92EduH1s7od2beohEQHpFsu4LqzaTgYLttFMZAF7DDtLGKWKHvaH3zb10FX3QTWGl64Kl+JXHhFB662+JaeLiNbA4XTayfwzxj3D9o3uAkcwZzpBZsEO6hLm32/IGbbSerbvi52U0odL4LalBhz4RUdLvdwDdqWNuk8DEV3v4AsYqYwmA5srF9N8fGBZkwv2CTY7dICb4JF2k4kgF2/zyQXHqy4MrooWOvKy1x4RY/fvcoCVK9VOg8L6Lpf0E6RJB1suTPW2wFV5bIQouUq2McfwvmidhrCV/ShI4C9G/WH3GJD+2h5Vml6F17RqnKvm4VJZCWE0YXrpQP0X5qG4B7apY28Y/gouA0KCtgr5lFLapkF2PX2sRRwq9Q1VX525ySnE68olt0zcKCyrI7EQFug96nAPpUCHrBG9KMaH8r7I4vUQ6mAfaV8wUhtf+GDem9Ygl0srxEoWkqxLydeMSvgnm8H/WGlMXbw9dc4gcoSIhcQAlR6h3Gza/BqlH8K2OVyMGtqPTg5DqggGXaVmB8YDOhwOPGKomJjg5SWADI7+1BKKhF9L2gdWBB8HHZ1Si3rTxWwh+o3TJQK3RkN+8xc7b5YQgzWjVfMgzmfSwBhN7t0HoxT3f8ERq2wpkGFMIO6u484Cl8B+8gSXCR32K3KzIt3u268fjReA9aTHezcC4Au0eCQfJPV0U4qzNSSAnbrXR0ytSy5wT472kzcrF+cbryiSnH24BiZrScOdshLECMTprekQUp+P7GSFLCP2NYh0idgn8WhxV6avmTOjVdM/kyIfDVe8RAQHr3aGSGPrjuJNQ9ySYzbbkdff/CPwt4caqC7fq+nkzuvxKabsgcunO/TZb/B3QX2QTw82Fag3kzI0jAH4cu0CHCz+eeF/Ad0e0/V3bhD5ubOK4qVKTm4zpnetNCPteRj9tvgkQLAMLtr0sjOOErXPGwifsCd2aS7euOonfcfgX3WIF9ofdB96cwrKvcpcToImKL7ZFWGi6IGvNIBHxDnw/QUNubqtpslaXA/elKzFg6cP2EoPgb7rLmlQ3EIT9cvz5VXdPsX4w8QJVWgoJasonSKjTAgv95CA75DJyfvvy7S/FSvaODeDDuOxZQLcD4Ie0OHMFP5J0tXXrfWJSEskeASKFkr8xAjksA6bGB/u2rwHRKtkoPZURDy55GZdTtOQ1MlIEcfhr1l6c5C7+9ceUUhaXu49JswYza/gv61EjywJ4dk7MB1v0jfuZImBCO+qNWpOTA4LVIxte0QAH0B7A2tTrJ5H7ryitJiM3bTK9nxthybbwd4SQQGWj1JTJJMNk1UR9r6Q9lt0CVep9g5XwR7w2koGK6ZK6/k4NixERvCzGVkdU2sqkaBtd1PBxBJJIRMvFf9pRe4PFSwQ3emJKa+DvaZGMO7uvJKtj/645Y7SQOlahx5QvVEq1FAk7dSHgwQ6rTjUBgOwkfjUwU7qowJGYovhV2IT3iOvNKjDcadME0mYDi2clZdXg0Top0PIPVJHAgLzjeGvmN8QwU7ugUTTk7+WtjpjT4XR14Fz3fMQZQkC5TsqOAwRuVRu+wF23uYTxHl0CcP4nYMk3jBXZ5195MEO66Aq7IlJU2DPa5WZXh6ZOnVN/g/ON5HR16FQo0Rt0fQQ2OaaYuC1LgrRpcOgKX5lPI7OAtI9ZhpmuE++JfIkHfFjIpZVpvkWmTBKSyPB4coHR7GoxeRiPTZkdeZcO6IdW1VTOy51iog5xaP2JwkiTpw3W9kgtDIAlp0htpycraPEnbUO0ZDCbVrO+kmCnnrWiwMZp8deZ3Rmjb74w2oy9ypF9QXkX7qkvCahNkwEwtsVaivw57rVfuFeHp98E+GnQQdDemkAzS5cYnJg6mm11RoylwceRXYmNtaGfRorEXXlv2dBJX+BoJhgW92IEME1pAH7ULZ0QoGJexEBPn6mYSGdSciJ8KOdeNaTwodp60jr23/aZlCYBGbFw5Eq/ufkRXddUP0NAt5swO47msw3ITOoZDXTdatkJvtJyQDO7FSI12wm2Q+O906EXYUttrlDrI0cuW1JeHE09Tkvu+EvNd7BpHCX9uzaxImzjLI73z4p2j54dcW6mCNlJHvpwgD+45EwAv1WJbkuKDut6kOHLNhh6MLfDJw5bUjAUbDjc4roepruNGZnlTlK9a7gAOXnB/UxWJoUuSK6BTlcpcPOe+jE9yRRbQ0MVX5NeTAsHnd/TgVdlyMyjPW6GFbZ1deO9qJQ8PdjvB69iFkBvYgN2j9tnj0dkcCDvyFkUw9obQFingOCrMmvslV1L0o5WDf0jT3gkfhzl5wOxV2kkb0Fc4YOWes+6ILrz1dpPxeumbh8OQiVWK7CadQyhcebIVTKBXHUDBVQ7Liox9bygzH7FUivU5ijyMU9x0E8iK6CErjtUImR+no3oiAU7FnYn7dnXl90VGu40ke4sa73TqXH6NomM6clW7NUQjnSq4llNeBYJNca6rgDye+RKX3HPgzZ8WCzM2DztyzWM/z7v9k2IWqAV+8OyouKXhvO2Y6r28qufotv3iEx+bE4upSho+UeyQTpsZZegJPmJbAVGZQpCOzmTB/LMLqZ7fycuiOZs6VZUl9dp+HXdJ3z+kUhMe2A+VJvq5riGtOj8lLou3aHBTdHpK9Wp+kM6bf8386r4DXpL2zcrpz1IYNdTBYuk+BiyNN2xPUpwAUB4tL8kpL/oDwdNjjEefJkyU7mVeg46g2OuKwGFHDrTwpVajcaYgNv9qP1wMWf2dOqK4RkO0cNaE565CBO4z4JHHRp/KKZHfXBRB7hvII3CNdgEDYBMrHnW3Hy1+j1uhMIuVdMSvrsdygn+2SeGVMKwUJK2Uir4Ri6TYCLUWq/Edo14lMW/MpbOFWnFtip5oahwL61pny6puhDpb7KGlgwinfbqtiJfk4jVeBrPbfdbRZqlFbWezm4g+bByKsKM8tsRgvv/2SdFCp5h44MQzJU0QhcCuzsFu2mTwMk3gVKQ4t9xFm2nakmI5E8r0SIhH7Vp0QPpoYzjtOsZqunfnaWx/N2yn3YpzAsbqmMl/34/MrZQKvMsWhxYrPjMXZYqCAkvJ2WyDiumuer7TTfdgTDpZLG57V3/FquHGVuaLDuahqrZeRezaQM41XllaBVuJcl1ZFeysmttOzYbcRA6a/vjbvrJpim4DfbtMWZ5ludN6JlwtBuzkD7Ad2vNZqozp56AZ9LK8qWp3EY716Sk/29XZeKDeyKaTLm1QE2thU/LF6yIIuydfE+sDCqkZaWtzfvnowo+ln/C6Mj5RQXk5ySKvpinQNuRuvOrqsT3kRLfx2uPwkylQbjTQUr25BcfWbIdk0W9P4W78V7w7bNC02YR/CRxElm57VR83ckyRsUYX/q5v1ymWeXv2+3eIRrlQAQHN6jHYCH+Kfz/fg2ZNmyPb+IsqXoe1Rq3a8/gfELfO2gTNXMAAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7143BC3E-F055-2D49-BBE8-8FF7B7F4AC18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="7343775"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="AutoShape 11" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAfYAAABbCAMAAAC2wFcKAAAAY1BMVEX///8AjNHv+PwfmtcPk9R/xehvvuXP6fav2/EGj9L5/P6f1O4vodn7/f71+v0FjtIWltXh8frH5vWHyenA4/TX7fg8p9wrn9mTzuxTseBft+KW0OxHrN5zwOa43/Lo9fuo2O9Of94sAAARxUlEQVR4nO1d6ZqiOhBVRFwAxQ0FEXj/p7yyKKeSygKxb09/3fVrxoZQyUlqTzKbGcgrb0ERLfz5k/wkKvJbWZne+aMfTV6dX+cMXYP19rt5+wx5Q6cW383Lv0FeWOw5zDvy8+N3M/gJ+oOd0iX31Zh3FNXxd3PpTH+wI60yE+Yd8OV3M+pKf7APdLADvaHsh5t3f7C/aLvcWKM+nyfr7+bXif5g72kVjQC9oeVP1vB/sHd0H7PUO8p23830dPqDvaE4GA36k9Kfi/sf7E/acrbcJg3u5ergeV51OYePlHHmfy7uf7DPZrtCAnQRnMV43G6dSchnP1W//8E+iyXUi5KHs3qIFsDjf+b1U/QH+ywXRbcm/Cq59j80cPMH+43i6If6x0O64JOfGbf59bAfqcKODsYXEvJC9n8w+XH67bDvFhREi8TqiuL+I8X8b4edOuyB1TtHIuevP9Ga/+WwHwnqueVbIXmr/kL+vop+Oewp4ldYr1tiz//E5f67Ya8JfJ71exWpxfiBybhfDXuMFXP784g3iddXfBmDX0a/GvY1gmdnzvUUEwfA6PT9c/SrYUfN7tuL+IbuCPvpi/j7OvrNsK8coNui8x7xz8SrMCgi/+nu7f0kzZfluJk1nrzzLciiRfPF+eb5ySy4H/kkoR3s1XqZRUljx/hJlC3XYyOS8fGUpwt//3x/UQT3i/mNS/goomTffzG4Ha0L1O15RZ995GKfzZbwMmcM7mqmBjc6iV0v4a8WxkUMs60mf9mWAVvbP0+lb86sYL8s5faipQK6oavvoYjXmTgAi8dK17cyT+YibdKThQodw2uMXI3S7A0dXmw9uIl1eajqrlNabo04WoQNYJb4uBDO2jpvOaNogj2uVTVmKRuVlGDf3hYjXn9StZQx54fMkVdcaPPxmx7SuV+czqwMPYhJPULXGp99DH/wzRINGoaJujbWAUaCJDHAXvOCg2+rIRH2Ut1Ayi3C3VK7PeGqyY+N5RVl/AS7ZqVSVfHJVJdXwKtoYBgDADto+T1RL6n0AYZyooi0sBsbzCX5RmHfaWvUNrIZddRB1xI7WSbxilJotIxX08WiBHdzH56Hx43ZPAgvXV+/nTRbt5CuqCN1sIfGfUHzRFxEBPbKCIUgtGuL+lWfXRPjeT3g3z6XRivNjLQ9fwt0iPxsTHYl1AH1S4YtA+TpCvNeDbtdNen+Tt9C2A/GpStYMXfj8+0nZUE/hVfMp1hoVUu6Kb8uUPGyCiqY6oYSjwoWdofhCNSfgnJoSQn7zrbBJXkNYK/MqM/nN3h3bX68pb243ifximbXx8KrJ0tGnhS9cAfmDXzcpCe1tqNEw2CrYB8xjQjuA+xGCd+SP2ici514pC9N5zXif3YiO3HVU9GLGPAo9vqACLBcj//eU829lYgK9jHCA2XnAJ3lRBzMGKtp0hFdFZN4jdGM+FAOrZQ+t8jD86GptF8v5e71Gg5d95uu+cvwnN+KioOwUPZRW9pfdaX9QSQZe28bWgH7UnwhyW/lxfO8wzGUokGYu+JX7CIIj1Xz8l0OK7ws81p4JT/Vx6YHh0t5k+I9Z2deiUX3mTrISgw4ZMSIrE7i33tVDq67IswrdbSbMXS+X29iN6qb0P23+c/DLk7b/ExMbjEGtRi+x8FODoDY3oXwzcuqIxxmQvhEjMSAqzORV3wt0Q22PQlSp5BczZ3g0W86ZYWuuy5uDSN0Ft97esNcKCsO6VR7DSsLuyfUFcq8eNR0HgxyGXap94Iz38krCgMXnb6RIXtr96m8olrUrjFrohbp5s49Izj1vbKCHzVWBhSAdVDhNPNVYcaKfPEl5VnYyTjxfvLsSIb7jZMI+4bzSUKidLr2wRRY8MH3M7b91lJTeUXV8JGiZ1KzMU8UMAgbrzpewELXhAuhp+3k8GAdaGpEPOTrZRRxsK8QlasqAUKm0dslFGBX9J74OV2EDISRKk1TAl+vBTqZV5wuH9nSROoqE2WqibodXTcqLuYqElp+bT9RXulcESwTfWHMwY6MXdXWjodj+QpzUdg3qt6jWdvaGWBhqRNRYPu8rLDJvOKLWvvZlkiBliazsyUmfSn2QhkmBi3YTVxo56oNN6GA6Q0ABnbwE+aJLtlZgex8LXcKu3I8SaFyTDul9qY8X3xqOq84FobgmBWdrfrdsoJWVqdfMJ+qSjLC1Gj59fbCD0pCOdSvDAZ2FH/6WDWaYb0pRWDXmEqp8Cqwplkponpz4BUZqLVv2hGGKVL9o0QdtDigAFd0AzR5F7oHCzLRl2xXMkwy7FtAzmTrwJLp9SOBXQMEavcGZ1BUmtgJYFc48oqwfyBag5wojZMX4bc7wQDqS9EPmCudFoQZb7JNgLeeNRl2DJuY6lkAhkT6gjaJjTJxzfWKJW/fnP76uNXni+fIKyr7MaXSFv0xRvhL6WFwwRVpOJi13WraXY71bZk3pWemGhHoqxJ2kFZmx2YhNoiw68xL+G6rmdDpta90ceD1w7CjtWnO4oL5t+9QBnZYRQ2C2iDSGQLp0o+tBDuqGbPwA0nTedIIu3Y04TNNPzHilFiUWDrzioL2A9l2aM4ClpP0cTm5pnxjfN4ImOsxkWBHcWM+kUdUtgj7RutVCNObZEb8m92EduH1s7od2beohEQHpFsu4LqzaTgYLttFMZAF7DDtLGKWKHvaH3zb10FX3QTWGl64Kl+JXHhFB662+JaeLiNbA4XTayfwzxj3D9o3uAkcwZzpBZsEO6hLm32/IGbbSerbvi52U0odL4LalBhz4RUdLvdwDdqWNuk8DEV3v4AsYqYwmA5srF9N8fGBZkwv2CTY7dICb4JF2k4kgF2/zyQXHqy4MrooWOvKy1x4RY/fvcoCVK9VOg8L6Lpf0E6RJB1suTPW2wFV5bIQouUq2McfwvmidhrCV/ShI4C9G/WH3GJD+2h5Vml6F17RqnKvm4VJZCWE0YXrpQP0X5qG4B7apY28Y/gouA0KCtgr5lFLapkF2PX2sRRwq9Q1VX525ySnE68olt0zcKCyrI7EQFug96nAPpUCHrBG9KMaH8r7I4vUQ6mAfaV8wUhtf+GDem9Ygl0srxEoWkqxLydeMSvgnm8H/WGlMXbw9dc4gcoSIhcQAlR6h3Gza/BqlH8K2OVyMGtqPTg5DqggGXaVmB8YDOhwOPGKomJjg5SWADI7+1BKKhF9L2gdWBB8HHZ1Si3rTxWwh+o3TJQK3RkN+8xc7b5YQgzWjVfMgzmfSwBhN7t0HoxT3f8ERq2wpkGFMIO6u484Cl8B+8gSXCR32K3KzIt3u268fjReA9aTHezcC4Au0eCQfJPV0U4qzNSSAnbrXR0ytSy5wT472kzcrF+cbryiSnH24BiZrScOdshLECMTprekQUp+P7GSFLCP2NYh0idgn8WhxV6avmTOjVdM/kyIfDVe8RAQHr3aGSGPrjuJNQ9ySYzbbkdff/CPwt4caqC7fq+nkzuvxKabsgcunO/TZb/B3QX2QTw82Fag3kzI0jAH4cu0CHCz+eeF/Ad0e0/V3bhD5ubOK4qVKTm4zpnetNCPteRj9tvgkQLAMLtr0sjOOErXPGwifsCd2aS7euOonfcfgX3WIF9ofdB96cwrKvcpcToImKL7ZFWGi6IGvNIBHxDnw/QUNubqtpslaXA/elKzFg6cP2EoPgb7rLmlQ3EIT9cvz5VXdPsX4w8QJVWgoJasonSKjTAgv95CA75DJyfvvy7S/FSvaODeDDuOxZQLcD4Ie0OHMFP5J0tXXrfWJSEskeASKFkr8xAjksA6bGB/u2rwHRKtkoPZURDy55GZdTtOQ1MlIEcfhr1l6c5C7+9ceUUhaXu49JswYza/gv61EjywJ4dk7MB1v0jfuZImBCO+qNWpOTA4LVIxte0QAH0B7A2tTrJ5H7ryitJiM3bTK9nxthybbwd4SQQGWj1JTJJMNk1UR9r6Q9lt0CVep9g5XwR7w2koGK6ZK6/k4NixERvCzGVkdU2sqkaBtd1PBxBJJIRMvFf9pRe4PFSwQ3emJKa+DvaZGMO7uvJKtj/645Y7SQOlahx5QvVEq1FAk7dSHgwQ6rTjUBgOwkfjUwU7qowJGYovhV2IT3iOvNKjDcadME0mYDi2clZdXg0Top0PIPVJHAgLzjeGvmN8QwU7ugUTTk7+WtjpjT4XR14Fz3fMQZQkC5TsqOAwRuVRu+wF23uYTxHl0CcP4nYMk3jBXZ5195MEO66Aq7IlJU2DPa5WZXh6ZOnVN/g/ON5HR16FQo0Rt0fQQ2OaaYuC1LgrRpcOgKX5lPI7OAtI9ZhpmuE++JfIkHfFjIpZVpvkWmTBKSyPB4coHR7GoxeRiPTZkdeZcO6IdW1VTOy51iog5xaP2JwkiTpw3W9kgtDIAlp0htpycraPEnbUO0ZDCbVrO+kmCnnrWiwMZp8deZ3Rmjb74w2oy9ypF9QXkX7qkvCahNkwEwtsVaivw57rVfuFeHp98E+GnQQdDemkAzS5cYnJg6mm11RoylwceRXYmNtaGfRorEXXlv2dBJX+BoJhgW92IEME1pAH7ULZ0QoGJexEBPn6mYSGdSciJ8KOdeNaTwodp60jr23/aZlCYBGbFw5Eq/ufkRXddUP0NAt5swO47msw3ITOoZDXTdatkJvtJyQDO7FSI12wm2Q+O906EXYUttrlDrI0cuW1JeHE09Tkvu+EvNd7BpHCX9uzaxImzjLI73z4p2j54dcW6mCNlJHvpwgD+45EwAv1WJbkuKDut6kOHLNhh6MLfDJw5bUjAUbDjc4roepruNGZnlTlK9a7gAOXnB/UxWJoUuSK6BTlcpcPOe+jE9yRRbQ0MVX5NeTAsHnd/TgVdlyMyjPW6GFbZ1deO9qJQ8PdjvB69iFkBvYgN2j9tnj0dkcCDvyFkUw9obQFingOCrMmvslV1L0o5WDf0jT3gkfhzl5wOxV2kkb0Fc4YOWes+6ILrz1dpPxeumbh8OQiVWK7CadQyhcebIVTKBXHUDBVQ7Liox9bygzH7FUivU5ijyMU9x0E8iK6CErjtUImR+no3oiAU7FnYn7dnXl90VGu40ke4sa73TqXH6NomM6clW7NUQjnSq4llNeBYJNca6rgDye+RKX3HPgzZ8WCzM2DztyzWM/z7v9k2IWqAV+8OyouKXhvO2Y6r28qufotv3iEx+bE4upSho+UeyQTpsZZegJPmJbAVGZQpCOzmTB/LMLqZ7fycuiOZs6VZUl9dp+HXdJ3z+kUhMe2A+VJvq5riGtOj8lLou3aHBTdHpK9Wp+kM6bf8386r4DXpL2zcrpz1IYNdTBYuk+BiyNN2xPUpwAUB4tL8kpL/oDwdNjjEefJkyU7mVeg46g2OuKwGFHDrTwpVajcaYgNv9qP1wMWf2dOqK4RkO0cNaE565CBO4z4JHHRp/KKZHfXBRB7hvII3CNdgEDYBMrHnW3Hy1+j1uhMIuVdMSvrsdygn+2SeGVMKwUJK2Uir4Ri6TYCLUWq/Edo14lMW/MpbOFWnFtip5oahwL61pny6puhDpb7KGlgwinfbqtiJfk4jVeBrPbfdbRZqlFbWezm4g+bByKsKM8tsRgvv/2SdFCp5h44MQzJU0QhcCuzsFu2mTwMk3gVKQ4t9xFm2nakmI5E8r0SIhH7Vp0QPpoYzjtOsZqunfnaWx/N2yn3YpzAsbqmMl/34/MrZQKvMsWhxYrPjMXZYqCAkvJ2WyDiumuer7TTfdgTDpZLG57V3/FquHGVuaLDuahqrZeRezaQM41XllaBVuJcl1ZFeysmttOzYbcRA6a/vjbvrJpim4DfbtMWZ5ludN6JlwtBuzkD7Ad2vNZqozp56AZ9LK8qWp3EY716Sk/29XZeKDeyKaTLm1QE2thU/LF6yIIuydfE+sDCqkZaWtzfvnowo+ln/C6Mj5RQXk5ySKvpinQNuRuvOrqsT3kRLfx2uPwkylQbjTQUr25BcfWbIdk0W9P4W78V7w7bNC02YR/CRxElm57VR83ckyRsUYX/q5v1ymWeXv2+3eIRrlQAQHN6jHYCH+Kfz/fg2ZNmyPb+IsqXoe1Rq3a8/gfELfO2gTNXMAAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF90F5E3-8A49-874F-B1E8-1B6D9CEA27C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="7343775"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="AutoShape 12" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAfYAAABbCAMAAAC2wFcKAAAAY1BMVEX///8AjNHv+PwfmtcPk9R/xehvvuXP6fav2/EGj9L5/P6f1O4vodn7/f71+v0FjtIWltXh8frH5vWHyenA4/TX7fg8p9wrn9mTzuxTseBft+KW0OxHrN5zwOa43/Lo9fuo2O9Of94sAAARxUlEQVR4nO1d6ZqiOhBVRFwAxQ0FEXj/p7yyKKeSygKxb09/3fVrxoZQyUlqTzKbGcgrb0ERLfz5k/wkKvJbWZne+aMfTV6dX+cMXYP19rt5+wx5Q6cW383Lv0FeWOw5zDvy8+N3M/gJ+oOd0iX31Zh3FNXxd3PpTH+wI60yE+Yd8OV3M+pKf7APdLADvaHsh5t3f7C/aLvcWKM+nyfr7+bXif5g72kVjQC9oeVP1vB/sHd0H7PUO8p23830dPqDvaE4GA36k9Kfi/sf7E/acrbcJg3u5ergeV51OYePlHHmfy7uf7DPZrtCAnQRnMV43G6dSchnP1W//8E+iyXUi5KHs3qIFsDjf+b1U/QH+ywXRbcm/Cq59j80cPMH+43i6If6x0O64JOfGbf59bAfqcKODsYXEvJC9n8w+XH67bDvFhREi8TqiuL+I8X8b4edOuyB1TtHIuevP9Ga/+WwHwnqueVbIXmr/kL+vop+Oewp4ldYr1tiz//E5f67Ya8JfJ71exWpxfiBybhfDXuMFXP784g3iddXfBmDX0a/GvY1gmdnzvUUEwfA6PT9c/SrYUfN7tuL+IbuCPvpi/j7OvrNsK8coNui8x7xz8SrMCgi/+nu7f0kzZfluJk1nrzzLciiRfPF+eb5ySy4H/kkoR3s1XqZRUljx/hJlC3XYyOS8fGUpwt//3x/UQT3i/mNS/goomTffzG4Ha0L1O15RZ995GKfzZbwMmcM7mqmBjc6iV0v4a8WxkUMs60mf9mWAVvbP0+lb86sYL8s5faipQK6oavvoYjXmTgAi8dK17cyT+YibdKThQodw2uMXI3S7A0dXmw9uIl1eajqrlNabo04WoQNYJb4uBDO2jpvOaNogj2uVTVmKRuVlGDf3hYjXn9StZQx54fMkVdcaPPxmx7SuV+czqwMPYhJPULXGp99DH/wzRINGoaJujbWAUaCJDHAXvOCg2+rIRH2Ut1Ayi3C3VK7PeGqyY+N5RVl/AS7ZqVSVfHJVJdXwKtoYBgDADto+T1RL6n0AYZyooi0sBsbzCX5RmHfaWvUNrIZddRB1xI7WSbxilJotIxX08WiBHdzH56Hx43ZPAgvXV+/nTRbt5CuqCN1sIfGfUHzRFxEBPbKCIUgtGuL+lWfXRPjeT3g3z6XRivNjLQ9fwt0iPxsTHYl1AH1S4YtA+TpCvNeDbtdNen+Tt9C2A/GpStYMXfj8+0nZUE/hVfMp1hoVUu6Kb8uUPGyCiqY6oYSjwoWdofhCNSfgnJoSQn7zrbBJXkNYK/MqM/nN3h3bX68pb243ifximbXx8KrJ0tGnhS9cAfmDXzcpCe1tqNEw2CrYB8xjQjuA+xGCd+SP2ici514pC9N5zXif3YiO3HVU9GLGPAo9vqACLBcj//eU829lYgK9jHCA2XnAJ3lRBzMGKtp0hFdFZN4jdGM+FAOrZQ+t8jD86GptF8v5e71Gg5d95uu+cvwnN+KioOwUPZRW9pfdaX9QSQZe28bWgH7UnwhyW/lxfO8wzGUokGYu+JX7CIIj1Xz8l0OK7ws81p4JT/Vx6YHh0t5k+I9Z2deiUX3mTrISgw4ZMSIrE7i33tVDq67IswrdbSbMXS+X29iN6qb0P23+c/DLk7b/ExMbjEGtRi+x8FODoDY3oXwzcuqIxxmQvhEjMSAqzORV3wt0Q22PQlSp5BczZ3g0W86ZYWuuy5uDSN0Ft97esNcKCsO6VR7DSsLuyfUFcq8eNR0HgxyGXap94Iz38krCgMXnb6RIXtr96m8olrUrjFrohbp5s49Izj1vbKCHzVWBhSAdVDhNPNVYcaKfPEl5VnYyTjxfvLsSIb7jZMI+4bzSUKidLr2wRRY8MH3M7b91lJTeUXV8JGiZ1KzMU8UMAgbrzpewELXhAuhp+3k8GAdaGpEPOTrZRRxsK8QlasqAUKm0dslFGBX9J74OV2EDISRKk1TAl+vBTqZV5wuH9nSROoqE2WqibodXTcqLuYqElp+bT9RXulcESwTfWHMwY6MXdXWjodj+QpzUdg3qt6jWdvaGWBhqRNRYPu8rLDJvOKLWvvZlkiBliazsyUmfSn2QhkmBi3YTVxo56oNN6GA6Q0ABnbwE+aJLtlZgex8LXcKu3I8SaFyTDul9qY8X3xqOq84FobgmBWdrfrdsoJWVqdfMJ+qSjLC1Gj59fbCD0pCOdSvDAZ2FH/6WDWaYb0pRWDXmEqp8Cqwplkponpz4BUZqLVv2hGGKVL9o0QdtDigAFd0AzR5F7oHCzLRl2xXMkwy7FtAzmTrwJLp9SOBXQMEavcGZ1BUmtgJYFc48oqwfyBag5wojZMX4bc7wQDqS9EPmCudFoQZb7JNgLeeNRl2DJuY6lkAhkT6gjaJjTJxzfWKJW/fnP76uNXni+fIKyr7MaXSFv0xRvhL6WFwwRVpOJi13WraXY71bZk3pWemGhHoqxJ2kFZmx2YhNoiw68xL+G6rmdDpta90ceD1w7CjtWnO4oL5t+9QBnZYRQ2C2iDSGQLp0o+tBDuqGbPwA0nTedIIu3Y04TNNPzHilFiUWDrzioL2A9l2aM4ClpP0cTm5pnxjfN4ImOsxkWBHcWM+kUdUtgj7RutVCNObZEb8m92EduH1s7od2beohEQHpFsu4LqzaTgYLttFMZAF7DDtLGKWKHvaH3zb10FX3QTWGl64Kl+JXHhFB662+JaeLiNbA4XTayfwzxj3D9o3uAkcwZzpBZsEO6hLm32/IGbbSerbvi52U0odL4LalBhz4RUdLvdwDdqWNuk8DEV3v4AsYqYwmA5srF9N8fGBZkwv2CTY7dICb4JF2k4kgF2/zyQXHqy4MrooWOvKy1x4RY/fvcoCVK9VOg8L6Lpf0E6RJB1suTPW2wFV5bIQouUq2McfwvmidhrCV/ShI4C9G/WH3GJD+2h5Vml6F17RqnKvm4VJZCWE0YXrpQP0X5qG4B7apY28Y/gouA0KCtgr5lFLapkF2PX2sRRwq9Q1VX525ySnE68olt0zcKCyrI7EQFug96nAPpUCHrBG9KMaH8r7I4vUQ6mAfaV8wUhtf+GDem9Ygl0srxEoWkqxLydeMSvgnm8H/WGlMXbw9dc4gcoSIhcQAlR6h3Gza/BqlH8K2OVyMGtqPTg5DqggGXaVmB8YDOhwOPGKomJjg5SWADI7+1BKKhF9L2gdWBB8HHZ1Si3rTxWwh+o3TJQK3RkN+8xc7b5YQgzWjVfMgzmfSwBhN7t0HoxT3f8ERq2wpkGFMIO6u484Cl8B+8gSXCR32K3KzIt3u268fjReA9aTHezcC4Au0eCQfJPV0U4qzNSSAnbrXR0ytSy5wT472kzcrF+cbryiSnH24BiZrScOdshLECMTprekQUp+P7GSFLCP2NYh0idgn8WhxV6avmTOjVdM/kyIfDVe8RAQHr3aGSGPrjuJNQ9ySYzbbkdff/CPwt4caqC7fq+nkzuvxKabsgcunO/TZb/B3QX2QTw82Fag3kzI0jAH4cu0CHCz+eeF/Ad0e0/V3bhD5ubOK4qVKTm4zpnetNCPteRj9tvgkQLAMLtr0sjOOErXPGwifsCd2aS7euOonfcfgX3WIF9ofdB96cwrKvcpcToImKL7ZFWGi6IGvNIBHxDnw/QUNubqtpslaXA/elKzFg6cP2EoPgb7rLmlQ3EIT9cvz5VXdPsX4w8QJVWgoJasonSKjTAgv95CA75DJyfvvy7S/FSvaODeDDuOxZQLcD4Ie0OHMFP5J0tXXrfWJSEskeASKFkr8xAjksA6bGB/u2rwHRKtkoPZURDy55GZdTtOQ1MlIEcfhr1l6c5C7+9ceUUhaXu49JswYza/gv61EjywJ4dk7MB1v0jfuZImBCO+qNWpOTA4LVIxte0QAH0B7A2tTrJ5H7ryitJiM3bTK9nxthybbwd4SQQGWj1JTJJMNk1UR9r6Q9lt0CVep9g5XwR7w2koGK6ZK6/k4NixERvCzGVkdU2sqkaBtd1PBxBJJIRMvFf9pRe4PFSwQ3emJKa+DvaZGMO7uvJKtj/645Y7SQOlahx5QvVEq1FAk7dSHgwQ6rTjUBgOwkfjUwU7qowJGYovhV2IT3iOvNKjDcadME0mYDi2clZdXg0Top0PIPVJHAgLzjeGvmN8QwU7ugUTTk7+WtjpjT4XR14Fz3fMQZQkC5TsqOAwRuVRu+wF23uYTxHl0CcP4nYMk3jBXZ5195MEO66Aq7IlJU2DPa5WZXh6ZOnVN/g/ON5HR16FQo0Rt0fQQ2OaaYuC1LgrRpcOgKX5lPI7OAtI9ZhpmuE++JfIkHfFjIpZVpvkWmTBKSyPB4coHR7GoxeRiPTZkdeZcO6IdW1VTOy51iog5xaP2JwkiTpw3W9kgtDIAlp0htpycraPEnbUO0ZDCbVrO+kmCnnrWiwMZp8deZ3Rmjb74w2oy9ypF9QXkX7qkvCahNkwEwtsVaivw57rVfuFeHp98E+GnQQdDemkAzS5cYnJg6mm11RoylwceRXYmNtaGfRorEXXlv2dBJX+BoJhgW92IEME1pAH7ULZ0QoGJexEBPn6mYSGdSciJ8KOdeNaTwodp60jr23/aZlCYBGbFw5Eq/ufkRXddUP0NAt5swO47msw3ITOoZDXTdatkJvtJyQDO7FSI12wm2Q+O906EXYUttrlDrI0cuW1JeHE09Tkvu+EvNd7BpHCX9uzaxImzjLI73z4p2j54dcW6mCNlJHvpwgD+45EwAv1WJbkuKDut6kOHLNhh6MLfDJw5bUjAUbDjc4roepruNGZnlTlK9a7gAOXnB/UxWJoUuSK6BTlcpcPOe+jE9yRRbQ0MVX5NeTAsHnd/TgVdlyMyjPW6GFbZ1deO9qJQ8PdjvB69iFkBvYgN2j9tnj0dkcCDvyFkUw9obQFingOCrMmvslV1L0o5WDf0jT3gkfhzl5wOxV2kkb0Fc4YOWes+6ILrz1dpPxeumbh8OQiVWK7CadQyhcebIVTKBXHUDBVQ7Liox9bygzH7FUivU5ijyMU9x0E8iK6CErjtUImR+no3oiAU7FnYn7dnXl90VGu40ke4sa73TqXH6NomM6clW7NUQjnSq4llNeBYJNca6rgDye+RKX3HPgzZ8WCzM2DztyzWM/z7v9k2IWqAV+8OyouKXhvO2Y6r28qufotv3iEx+bE4upSho+UeyQTpsZZegJPmJbAVGZQpCOzmTB/LMLqZ7fycuiOZs6VZUl9dp+HXdJ3z+kUhMe2A+VJvq5riGtOj8lLou3aHBTdHpK9Wp+kM6bf8386r4DXpL2zcrpz1IYNdTBYuk+BiyNN2xPUpwAUB4tL8kpL/oDwdNjjEefJkyU7mVeg46g2OuKwGFHDrTwpVajcaYgNv9qP1wMWf2dOqK4RkO0cNaE565CBO4z4JHHRp/KKZHfXBRB7hvII3CNdgEDYBMrHnW3Hy1+j1uhMIuVdMSvrsdygn+2SeGVMKwUJK2Uir4Ri6TYCLUWq/Edo14lMW/MpbOFWnFtip5oahwL61pny6puhDpb7KGlgwinfbqtiJfk4jVeBrPbfdbRZqlFbWezm4g+bByKsKM8tsRgvv/2SdFCp5h44MQzJU0QhcCuzsFu2mTwMk3gVKQ4t9xFm2nakmI5E8r0SIhH7Vp0QPpoYzjtOsZqunfnaWx/N2yn3YpzAsbqmMl/34/MrZQKvMsWhxYrPjMXZYqCAkvJ2WyDiumuer7TTfdgTDpZLG57V3/FquHGVuaLDuahqrZeRezaQM41XllaBVuJcl1ZFeysmttOzYbcRA6a/vjbvrJpim4DfbtMWZ5ludN6JlwtBuzkD7Ad2vNZqozp56AZ9LK8qWp3EY716Sk/29XZeKDeyKaTLm1QE2thU/LF6yIIuydfE+sDCqkZaWtzfvnowo+ln/C6Mj5RQXk5ySKvpinQNuRuvOrqsT3kRLfx2uPwkylQbjTQUr25BcfWbIdk0W9P4W78V7w7bNC02YR/CRxElm57VR83ckyRsUYX/q5v1ymWeXv2+3eIRrlQAQHN6jHYCH+Kfz/fg2ZNmyPb+IsqXoe1Rq3a8/gfELfO2gTNXMAAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEA98681-87AE-964A-89C9-AEC67FE16B87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="7343775"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="AutoShape 11" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAfYAAABbCAMAAAC2wFcKAAAAY1BMVEX///8AjNHv+PwfmtcPk9R/xehvvuXP6fav2/EGj9L5/P6f1O4vodn7/f71+v0FjtIWltXh8frH5vWHyenA4/TX7fg8p9wrn9mTzuxTseBft+KW0OxHrN5zwOa43/Lo9fuo2O9Of94sAAARxUlEQVR4nO1d6ZqiOhBVRFwAxQ0FEXj/p7yyKKeSygKxb09/3fVrxoZQyUlqTzKbGcgrb0ERLfz5k/wkKvJbWZne+aMfTV6dX+cMXYP19rt5+wx5Q6cW383Lv0FeWOw5zDvy8+N3M/gJ+oOd0iX31Zh3FNXxd3PpTH+wI60yE+Yd8OV3M+pKf7APdLADvaHsh5t3f7C/aLvcWKM+nyfr7+bXif5g72kVjQC9oeVP1vB/sHd0H7PUO8p23830dPqDvaE4GA36k9Kfi/sf7E/acrbcJg3u5ergeV51OYePlHHmfy7uf7DPZrtCAnQRnMV43G6dSchnP1W//8E+iyXUi5KHs3qIFsDjf+b1U/QH+ywXRbcm/Cq59j80cPMH+43i6If6x0O64JOfGbf59bAfqcKODsYXEvJC9n8w+XH67bDvFhREi8TqiuL+I8X8b4edOuyB1TtHIuevP9Ga/+WwHwnqueVbIXmr/kL+vop+Oewp4ldYr1tiz//E5f67Ya8JfJ71exWpxfiBybhfDXuMFXP784g3iddXfBmDX0a/GvY1gmdnzvUUEwfA6PT9c/SrYUfN7tuL+IbuCPvpi/j7OvrNsK8coNui8x7xz8SrMCgi/+nu7f0kzZfluJk1nrzzLciiRfPF+eb5ySy4H/kkoR3s1XqZRUljx/hJlC3XYyOS8fGUpwt//3x/UQT3i/mNS/goomTffzG4Ha0L1O15RZ995GKfzZbwMmcM7mqmBjc6iV0v4a8WxkUMs60mf9mWAVvbP0+lb86sYL8s5faipQK6oavvoYjXmTgAi8dK17cyT+YibdKThQodw2uMXI3S7A0dXmw9uIl1eajqrlNabo04WoQNYJb4uBDO2jpvOaNogj2uVTVmKRuVlGDf3hYjXn9StZQx54fMkVdcaPPxmx7SuV+czqwMPYhJPULXGp99DH/wzRINGoaJujbWAUaCJDHAXvOCg2+rIRH2Ut1Ayi3C3VK7PeGqyY+N5RVl/AS7ZqVSVfHJVJdXwKtoYBgDADto+T1RL6n0AYZyooi0sBsbzCX5RmHfaWvUNrIZddRB1xI7WSbxilJotIxX08WiBHdzH56Hx43ZPAgvXV+/nTRbt5CuqCN1sIfGfUHzRFxEBPbKCIUgtGuL+lWfXRPjeT3g3z6XRivNjLQ9fwt0iPxsTHYl1AH1S4YtA+TpCvNeDbtdNen+Tt9C2A/GpStYMXfj8+0nZUE/hVfMp1hoVUu6Kb8uUPGyCiqY6oYSjwoWdofhCNSfgnJoSQn7zrbBJXkNYK/MqM/nN3h3bX68pb243ifximbXx8KrJ0tGnhS9cAfmDXzcpCe1tqNEw2CrYB8xjQjuA+xGCd+SP2ici514pC9N5zXif3YiO3HVU9GLGPAo9vqACLBcj//eU829lYgK9jHCA2XnAJ3lRBzMGKtp0hFdFZN4jdGM+FAOrZQ+t8jD86GptF8v5e71Gg5d95uu+cvwnN+KioOwUPZRW9pfdaX9QSQZe28bWgH7UnwhyW/lxfO8wzGUokGYu+JX7CIIj1Xz8l0OK7ws81p4JT/Vx6YHh0t5k+I9Z2deiUX3mTrISgw4ZMSIrE7i33tVDq67IswrdbSbMXS+X29iN6qb0P23+c/DLk7b/ExMbjEGtRi+x8FODoDY3oXwzcuqIxxmQvhEjMSAqzORV3wt0Q22PQlSp5BczZ3g0W86ZYWuuy5uDSN0Ft97esNcKCsO6VR7DSsLuyfUFcq8eNR0HgxyGXap94Iz38krCgMXnb6RIXtr96m8olrUrjFrohbp5s49Izj1vbKCHzVWBhSAdVDhNPNVYcaKfPEl5VnYyTjxfvLsSIb7jZMI+4bzSUKidLr2wRRY8MH3M7b91lJTeUXV8JGiZ1KzMU8UMAgbrzpewELXhAuhp+3k8GAdaGpEPOTrZRRxsK8QlasqAUKm0dslFGBX9J74OV2EDISRKk1TAl+vBTqZV5wuH9nSROoqE2WqibodXTcqLuYqElp+bT9RXulcESwTfWHMwY6MXdXWjodj+QpzUdg3qt6jWdvaGWBhqRNRYPu8rLDJvOKLWvvZlkiBliazsyUmfSn2QhkmBi3YTVxo56oNN6GA6Q0ABnbwE+aJLtlZgex8LXcKu3I8SaFyTDul9qY8X3xqOq84FobgmBWdrfrdsoJWVqdfMJ+qSjLC1Gj59fbCD0pCOdSvDAZ2FH/6WDWaYb0pRWDXmEqp8Cqwplkponpz4BUZqLVv2hGGKVL9o0QdtDigAFd0AzR5F7oHCzLRl2xXMkwy7FtAzmTrwJLp9SOBXQMEavcGZ1BUmtgJYFc48oqwfyBag5wojZMX4bc7wQDqS9EPmCudFoQZb7JNgLeeNRl2DJuY6lkAhkT6gjaJjTJxzfWKJW/fnP76uNXni+fIKyr7MaXSFv0xRvhL6WFwwRVpOJi13WraXY71bZk3pWemGhHoqxJ2kFZmx2YhNoiw68xL+G6rmdDpta90ceD1w7CjtWnO4oL5t+9QBnZYRQ2C2iDSGQLp0o+tBDuqGbPwA0nTedIIu3Y04TNNPzHilFiUWDrzioL2A9l2aM4ClpP0cTm5pnxjfN4ImOsxkWBHcWM+kUdUtgj7RutVCNObZEb8m92EduH1s7od2beohEQHpFsu4LqzaTgYLttFMZAF7DDtLGKWKHvaH3zb10FX3QTWGl64Kl+JXHhFB662+JaeLiNbA4XTayfwzxj3D9o3uAkcwZzpBZsEO6hLm32/IGbbSerbvi52U0odL4LalBhz4RUdLvdwDdqWNuk8DEV3v4AsYqYwmA5srF9N8fGBZkwv2CTY7dICb4JF2k4kgF2/zyQXHqy4MrooWOvKy1x4RY/fvcoCVK9VOg8L6Lpf0E6RJB1suTPW2wFV5bIQouUq2McfwvmidhrCV/ShI4C9G/WH3GJD+2h5Vml6F17RqnKvm4VJZCWE0YXrpQP0X5qG4B7apY28Y/gouA0KCtgr5lFLapkF2PX2sRRwq9Q1VX525ySnE68olt0zcKCyrI7EQFug96nAPpUCHrBG9KMaH8r7I4vUQ6mAfaV8wUhtf+GDem9Ygl0srxEoWkqxLydeMSvgnm8H/WGlMXbw9dc4gcoSIhcQAlR6h3Gza/BqlH8K2OVyMGtqPTg5DqggGXaVmB8YDOhwOPGKomJjg5SWADI7+1BKKhF9L2gdWBB8HHZ1Si3rTxWwh+o3TJQK3RkN+8xc7b5YQgzWjVfMgzmfSwBhN7t0HoxT3f8ERq2wpkGFMIO6u484Cl8B+8gSXCR32K3KzIt3u268fjReA9aTHezcC4Au0eCQfJPV0U4qzNSSAnbrXR0ytSy5wT472kzcrF+cbryiSnH24BiZrScOdshLECMTprekQUp+P7GSFLCP2NYh0idgn8WhxV6avmTOjVdM/kyIfDVe8RAQHr3aGSGPrjuJNQ9ySYzbbkdff/CPwt4caqC7fq+nkzuvxKabsgcunO/TZb/B3QX2QTw82Fag3kzI0jAH4cu0CHCz+eeF/Ad0e0/V3bhD5ubOK4qVKTm4zpnetNCPteRj9tvgkQLAMLtr0sjOOErXPGwifsCd2aS7euOonfcfgX3WIF9ofdB96cwrKvcpcToImKL7ZFWGi6IGvNIBHxDnw/QUNubqtpslaXA/elKzFg6cP2EoPgb7rLmlQ3EIT9cvz5VXdPsX4w8QJVWgoJasonSKjTAgv95CA75DJyfvvy7S/FSvaODeDDuOxZQLcD4Ie0OHMFP5J0tXXrfWJSEskeASKFkr8xAjksA6bGB/u2rwHRKtkoPZURDy55GZdTtOQ1MlIEcfhr1l6c5C7+9ceUUhaXu49JswYza/gv61EjywJ4dk7MB1v0jfuZImBCO+qNWpOTA4LVIxte0QAH0B7A2tTrJ5H7ryitJiM3bTK9nxthybbwd4SQQGWj1JTJJMNk1UR9r6Q9lt0CVep9g5XwR7w2koGK6ZK6/k4NixERvCzGVkdU2sqkaBtd1PBxBJJIRMvFf9pRe4PFSwQ3emJKa+DvaZGMO7uvJKtj/645Y7SQOlahx5QvVEq1FAk7dSHgwQ6rTjUBgOwkfjUwU7qowJGYovhV2IT3iOvNKjDcadME0mYDi2clZdXg0Top0PIPVJHAgLzjeGvmN8QwU7ugUTTk7+WtjpjT4XR14Fz3fMQZQkC5TsqOAwRuVRu+wF23uYTxHl0CcP4nYMk3jBXZ5195MEO66Aq7IlJU2DPa5WZXh6ZOnVN/g/ON5HR16FQo0Rt0fQQ2OaaYuC1LgrRpcOgKX5lPI7OAtI9ZhpmuE++JfIkHfFjIpZVpvkWmTBKSyPB4coHR7GoxeRiPTZkdeZcO6IdW1VTOy51iog5xaP2JwkiTpw3W9kgtDIAlp0htpycraPEnbUO0ZDCbVrO+kmCnnrWiwMZp8deZ3Rmjb74w2oy9ypF9QXkX7qkvCahNkwEwtsVaivw57rVfuFeHp98E+GnQQdDemkAzS5cYnJg6mm11RoylwceRXYmNtaGfRorEXXlv2dBJX+BoJhgW92IEME1pAH7ULZ0QoGJexEBPn6mYSGdSciJ8KOdeNaTwodp60jr23/aZlCYBGbFw5Eq/ufkRXddUP0NAt5swO47msw3ITOoZDXTdatkJvtJyQDO7FSI12wm2Q+O906EXYUttrlDrI0cuW1JeHE09Tkvu+EvNd7BpHCX9uzaxImzjLI73z4p2j54dcW6mCNlJHvpwgD+45EwAv1WJbkuKDut6kOHLNhh6MLfDJw5bUjAUbDjc4roepruNGZnlTlK9a7gAOXnB/UxWJoUuSK6BTlcpcPOe+jE9yRRbQ0MVX5NeTAsHnd/TgVdlyMyjPW6GFbZ1deO9qJQ8PdjvB69iFkBvYgN2j9tnj0dkcCDvyFkUw9obQFingOCrMmvslV1L0o5WDf0jT3gkfhzl5wOxV2kkb0Fc4YOWes+6ILrz1dpPxeumbh8OQiVWK7CadQyhcebIVTKBXHUDBVQ7Liox9bygzH7FUivU5ijyMU9x0E8iK6CErjtUImR+no3oiAU7FnYn7dnXl90VGu40ke4sa73TqXH6NomM6clW7NUQjnSq4llNeBYJNca6rgDye+RKX3HPgzZ8WCzM2DztyzWM/z7v9k2IWqAV+8OyouKXhvO2Y6r28qufotv3iEx+bE4upSho+UeyQTpsZZegJPmJbAVGZQpCOzmTB/LMLqZ7fycuiOZs6VZUl9dp+HXdJ3z+kUhMe2A+VJvq5riGtOj8lLou3aHBTdHpK9Wp+kM6bf8386r4DXpL2zcrpz1IYNdTBYuk+BiyNN2xPUpwAUB4tL8kpL/oDwdNjjEefJkyU7mVeg46g2OuKwGFHDrTwpVajcaYgNv9qP1wMWf2dOqK4RkO0cNaE565CBO4z4JHHRp/KKZHfXBRB7hvII3CNdgEDYBMrHnW3Hy1+j1uhMIuVdMSvrsdygn+2SeGVMKwUJK2Uir4Ri6TYCLUWq/Edo14lMW/MpbOFWnFtip5oahwL61pny6puhDpb7KGlgwinfbqtiJfk4jVeBrPbfdbRZqlFbWezm4g+bByKsKM8tsRgvv/2SdFCp5h44MQzJU0QhcCuzsFu2mTwMk3gVKQ4t9xFm2nakmI5E8r0SIhH7Vp0QPpoYzjtOsZqunfnaWx/N2yn3YpzAsbqmMl/34/MrZQKvMsWhxYrPjMXZYqCAkvJ2WyDiumuer7TTfdgTDpZLG57V3/FquHGVuaLDuahqrZeRezaQM41XllaBVuJcl1ZFeysmttOzYbcRA6a/vjbvrJpim4DfbtMWZ5ludN6JlwtBuzkD7Ad2vNZqozp56AZ9LK8qWp3EY716Sk/29XZeKDeyKaTLm1QE2thU/LF6yIIuydfE+sDCqkZaWtzfvnowo+ln/C6Mj5RQXk5ySKvpinQNuRuvOrqsT3kRLfx2uPwkylQbjTQUr25BcfWbIdk0W9P4W78V7w7bNC02YR/CRxElm57VR83ckyRsUYX/q5v1ymWeXv2+3eIRrlQAQHN6jHYCH+Kfz/fg2ZNmyPb+IsqXoe1Rq3a8/gfELfO2gTNXMAAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9E9C0AB-8A28-0548-AD81-7BACB901917D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="7343775"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="AutoShape 12" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAfYAAABbCAMAAAC2wFcKAAAAY1BMVEX///8AjNHv+PwfmtcPk9R/xehvvuXP6fav2/EGj9L5/P6f1O4vodn7/f71+v0FjtIWltXh8frH5vWHyenA4/TX7fg8p9wrn9mTzuxTseBft+KW0OxHrN5zwOa43/Lo9fuo2O9Of94sAAARxUlEQVR4nO1d6ZqiOhBVRFwAxQ0FEXj/p7yyKKeSygKxb09/3fVrxoZQyUlqTzKbGcgrb0ERLfz5k/wkKvJbWZne+aMfTV6dX+cMXYP19rt5+wx5Q6cW383Lv0FeWOw5zDvy8+N3M/gJ+oOd0iX31Zh3FNXxd3PpTH+wI60yE+Yd8OV3M+pKf7APdLADvaHsh5t3f7C/aLvcWKM+nyfr7+bXif5g72kVjQC9oeVP1vB/sHd0H7PUO8p23830dPqDvaE4GA36k9Kfi/sf7E/acrbcJg3u5ergeV51OYePlHHmfy7uf7DPZrtCAnQRnMV43G6dSchnP1W//8E+iyXUi5KHs3qIFsDjf+b1U/QH+ywXRbcm/Cq59j80cPMH+43i6If6x0O64JOfGbf59bAfqcKODsYXEvJC9n8w+XH67bDvFhREi8TqiuL+I8X8b4edOuyB1TtHIuevP9Ga/+WwHwnqueVbIXmr/kL+vop+Oewp4ldYr1tiz//E5f67Ya8JfJ71exWpxfiBybhfDXuMFXP784g3iddXfBmDX0a/GvY1gmdnzvUUEwfA6PT9c/SrYUfN7tuL+IbuCPvpi/j7OvrNsK8coNui8x7xz8SrMCgi/+nu7f0kzZfluJk1nrzzLciiRfPF+eb5ySy4H/kkoR3s1XqZRUljx/hJlC3XYyOS8fGUpwt//3x/UQT3i/mNS/goomTffzG4Ha0L1O15RZ995GKfzZbwMmcM7mqmBjc6iV0v4a8WxkUMs60mf9mWAVvbP0+lb86sYL8s5faipQK6oavvoYjXmTgAi8dK17cyT+YibdKThQodw2uMXI3S7A0dXmw9uIl1eajqrlNabo04WoQNYJb4uBDO2jpvOaNogj2uVTVmKRuVlGDf3hYjXn9StZQx54fMkVdcaPPxmx7SuV+czqwMPYhJPULXGp99DH/wzRINGoaJujbWAUaCJDHAXvOCg2+rIRH2Ut1Ayi3C3VK7PeGqyY+N5RVl/AS7ZqVSVfHJVJdXwKtoYBgDADto+T1RL6n0AYZyooi0sBsbzCX5RmHfaWvUNrIZddRB1xI7WSbxilJotIxX08WiBHdzH56Hx43ZPAgvXV+/nTRbt5CuqCN1sIfGfUHzRFxEBPbKCIUgtGuL+lWfXRPjeT3g3z6XRivNjLQ9fwt0iPxsTHYl1AH1S4YtA+TpCvNeDbtdNen+Tt9C2A/GpStYMXfj8+0nZUE/hVfMp1hoVUu6Kb8uUPGyCiqY6oYSjwoWdofhCNSfgnJoSQn7zrbBJXkNYK/MqM/nN3h3bX68pb243ifximbXx8KrJ0tGnhS9cAfmDXzcpCe1tqNEw2CrYB8xjQjuA+xGCd+SP2ici514pC9N5zXif3YiO3HVU9GLGPAo9vqACLBcj//eU829lYgK9jHCA2XnAJ3lRBzMGKtp0hFdFZN4jdGM+FAOrZQ+t8jD86GptF8v5e71Gg5d95uu+cvwnN+KioOwUPZRW9pfdaX9QSQZe28bWgH7UnwhyW/lxfO8wzGUokGYu+JX7CIIj1Xz8l0OK7ws81p4JT/Vx6YHh0t5k+I9Z2deiUX3mTrISgw4ZMSIrE7i33tVDq67IswrdbSbMXS+X29iN6qb0P23+c/DLk7b/ExMbjEGtRi+x8FODoDY3oXwzcuqIxxmQvhEjMSAqzORV3wt0Q22PQlSp5BczZ3g0W86ZYWuuy5uDSN0Ft97esNcKCsO6VR7DSsLuyfUFcq8eNR0HgxyGXap94Iz38krCgMXnb6RIXtr96m8olrUrjFrohbp5s49Izj1vbKCHzVWBhSAdVDhNPNVYcaKfPEl5VnYyTjxfvLsSIb7jZMI+4bzSUKidLr2wRRY8MH3M7b91lJTeUXV8JGiZ1KzMU8UMAgbrzpewELXhAuhp+3k8GAdaGpEPOTrZRRxsK8QlasqAUKm0dslFGBX9J74OV2EDISRKk1TAl+vBTqZV5wuH9nSROoqE2WqibodXTcqLuYqElp+bT9RXulcESwTfWHMwY6MXdXWjodj+QpzUdg3qt6jWdvaGWBhqRNRYPu8rLDJvOKLWvvZlkiBliazsyUmfSn2QhkmBi3YTVxo56oNN6GA6Q0ABnbwE+aJLtlZgex8LXcKu3I8SaFyTDul9qY8X3xqOq84FobgmBWdrfrdsoJWVqdfMJ+qSjLC1Gj59fbCD0pCOdSvDAZ2FH/6WDWaYb0pRWDXmEqp8Cqwplkponpz4BUZqLVv2hGGKVL9o0QdtDigAFd0AzR5F7oHCzLRl2xXMkwy7FtAzmTrwJLp9SOBXQMEavcGZ1BUmtgJYFc48oqwfyBag5wojZMX4bc7wQDqS9EPmCudFoQZb7JNgLeeNRl2DJuY6lkAhkT6gjaJjTJxzfWKJW/fnP76uNXni+fIKyr7MaXSFv0xRvhL6WFwwRVpOJi13WraXY71bZk3pWemGhHoqxJ2kFZmx2YhNoiw68xL+G6rmdDpta90ceD1w7CjtWnO4oL5t+9QBnZYRQ2C2iDSGQLp0o+tBDuqGbPwA0nTedIIu3Y04TNNPzHilFiUWDrzioL2A9l2aM4ClpP0cTm5pnxjfN4ImOsxkWBHcWM+kUdUtgj7RutVCNObZEb8m92EduH1s7od2beohEQHpFsu4LqzaTgYLttFMZAF7DDtLGKWKHvaH3zb10FX3QTWGl64Kl+JXHhFB662+JaeLiNbA4XTayfwzxj3D9o3uAkcwZzpBZsEO6hLm32/IGbbSerbvi52U0odL4LalBhz4RUdLvdwDdqWNuk8DEV3v4AsYqYwmA5srF9N8fGBZkwv2CTY7dICb4JF2k4kgF2/zyQXHqy4MrooWOvKy1x4RY/fvcoCVK9VOg8L6Lpf0E6RJB1suTPW2wFV5bIQouUq2McfwvmidhrCV/ShI4C9G/WH3GJD+2h5Vml6F17RqnKvm4VJZCWE0YXrpQP0X5qG4B7apY28Y/gouA0KCtgr5lFLapkF2PX2sRRwq9Q1VX525ySnE68olt0zcKCyrI7EQFug96nAPpUCHrBG9KMaH8r7I4vUQ6mAfaV8wUhtf+GDem9Ygl0srxEoWkqxLydeMSvgnm8H/WGlMXbw9dc4gcoSIhcQAlR6h3Gza/BqlH8K2OVyMGtqPTg5DqggGXaVmB8YDOhwOPGKomJjg5SWADI7+1BKKhF9L2gdWBB8HHZ1Si3rTxWwh+o3TJQK3RkN+8xc7b5YQgzWjVfMgzmfSwBhN7t0HoxT3f8ERq2wpkGFMIO6u484Cl8B+8gSXCR32K3KzIt3u268fjReA9aTHezcC4Au0eCQfJPV0U4qzNSSAnbrXR0ytSy5wT472kzcrF+cbryiSnH24BiZrScOdshLECMTprekQUp+P7GSFLCP2NYh0idgn8WhxV6avmTOjVdM/kyIfDVe8RAQHr3aGSGPrjuJNQ9ySYzbbkdff/CPwt4caqC7fq+nkzuvxKabsgcunO/TZb/B3QX2QTw82Fag3kzI0jAH4cu0CHCz+eeF/Ad0e0/V3bhD5ubOK4qVKTm4zpnetNCPteRj9tvgkQLAMLtr0sjOOErXPGwifsCd2aS7euOonfcfgX3WIF9ofdB96cwrKvcpcToImKL7ZFWGi6IGvNIBHxDnw/QUNubqtpslaXA/elKzFg6cP2EoPgb7rLmlQ3EIT9cvz5VXdPsX4w8QJVWgoJasonSKjTAgv95CA75DJyfvvy7S/FSvaODeDDuOxZQLcD4Ie0OHMFP5J0tXXrfWJSEskeASKFkr8xAjksA6bGB/u2rwHRKtkoPZURDy55GZdTtOQ1MlIEcfhr1l6c5C7+9ceUUhaXu49JswYza/gv61EjywJ4dk7MB1v0jfuZImBCO+qNWpOTA4LVIxte0QAH0B7A2tTrJ5H7ryitJiM3bTK9nxthybbwd4SQQGWj1JTJJMNk1UR9r6Q9lt0CVep9g5XwR7w2koGK6ZK6/k4NixERvCzGVkdU2sqkaBtd1PBxBJJIRMvFf9pRe4PFSwQ3emJKa+DvaZGMO7uvJKtj/645Y7SQOlahx5QvVEq1FAk7dSHgwQ6rTjUBgOwkfjUwU7qowJGYovhV2IT3iOvNKjDcadME0mYDi2clZdXg0Top0PIPVJHAgLzjeGvmN8QwU7ugUTTk7+WtjpjT4XR14Fz3fMQZQkC5TsqOAwRuVRu+wF23uYTxHl0CcP4nYMk3jBXZ5195MEO66Aq7IlJU2DPa5WZXh6ZOnVN/g/ON5HR16FQo0Rt0fQQ2OaaYuC1LgrRpcOgKX5lPI7OAtI9ZhpmuE++JfIkHfFjIpZVpvkWmTBKSyPB4coHR7GoxeRiPTZkdeZcO6IdW1VTOy51iog5xaP2JwkiTpw3W9kgtDIAlp0htpycraPEnbUO0ZDCbVrO+kmCnnrWiwMZp8deZ3Rmjb74w2oy9ypF9QXkX7qkvCahNkwEwtsVaivw57rVfuFeHp98E+GnQQdDemkAzS5cYnJg6mm11RoylwceRXYmNtaGfRorEXXlv2dBJX+BoJhgW92IEME1pAH7ULZ0QoGJexEBPn6mYSGdSciJ8KOdeNaTwodp60jr23/aZlCYBGbFw5Eq/ufkRXddUP0NAt5swO47msw3ITOoZDXTdatkJvtJyQDO7FSI12wm2Q+O906EXYUttrlDrI0cuW1JeHE09Tkvu+EvNd7BpHCX9uzaxImzjLI73z4p2j54dcW6mCNlJHvpwgD+45EwAv1WJbkuKDut6kOHLNhh6MLfDJw5bUjAUbDjc4roepruNGZnlTlK9a7gAOXnB/UxWJoUuSK6BTlcpcPOe+jE9yRRbQ0MVX5NeTAsHnd/TgVdlyMyjPW6GFbZ1deO9qJQ8PdjvB69iFkBvYgN2j9tnj0dkcCDvyFkUw9obQFingOCrMmvslV1L0o5WDf0jT3gkfhzl5wOxV2kkb0Fc4YOWes+6ILrz1dpPxeumbh8OQiVWK7CadQyhcebIVTKBXHUDBVQ7Liox9bygzH7FUivU5ijyMU9x0E8iK6CErjtUImR+no3oiAU7FnYn7dnXl90VGu40ke4sa73TqXH6NomM6clW7NUQjnSq4llNeBYJNca6rgDye+RKX3HPgzZ8WCzM2DztyzWM/z7v9k2IWqAV+8OyouKXhvO2Y6r28qufotv3iEx+bE4upSho+UeyQTpsZZegJPmJbAVGZQpCOzmTB/LMLqZ7fycuiOZs6VZUl9dp+HXdJ3z+kUhMe2A+VJvq5riGtOj8lLou3aHBTdHpK9Wp+kM6bf8386r4DXpL2zcrpz1IYNdTBYuk+BiyNN2xPUpwAUB4tL8kpL/oDwdNjjEefJkyU7mVeg46g2OuKwGFHDrTwpVajcaYgNv9qP1wMWf2dOqK4RkO0cNaE565CBO4z4JHHRp/KKZHfXBRB7hvII3CNdgEDYBMrHnW3Hy1+j1uhMIuVdMSvrsdygn+2SeGVMKwUJK2Uir4Ri6TYCLUWq/Edo14lMW/MpbOFWnFtip5oahwL61pny6puhDpb7KGlgwinfbqtiJfk4jVeBrPbfdbRZqlFbWezm4g+bByKsKM8tsRgvv/2SdFCp5h44MQzJU0QhcCuzsFu2mTwMk3gVKQ4t9xFm2nakmI5E8r0SIhH7Vp0QPpoYzjtOsZqunfnaWx/N2yn3YpzAsbqmMl/34/MrZQKvMsWhxYrPjMXZYqCAkvJ2WyDiumuer7TTfdgTDpZLG57V3/FquHGVuaLDuahqrZeRezaQM41XllaBVuJcl1ZFeysmttOzYbcRA6a/vjbvrJpim4DfbtMWZ5ludN6JlwtBuzkD7Ad2vNZqozp56AZ9LK8qWp3EY716Sk/29XZeKDeyKaTLm1QE2thU/LF6yIIuydfE+sDCqkZaWtzfvnowo+ln/C6Mj5RQXk5ySKvpinQNuRuvOrqsT3kRLfx2uPwkylQbjTQUr25BcfWbIdk0W9P4W78V7w7bNC02YR/CRxElm57VR83ckyRsUYX/q5v1ymWeXv2+3eIRrlQAQHN6jHYCH+Kfz/fg2ZNmyPb+IsqXoe1Rq3a8/gfELfO2gTNXMAAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31DE808B-AF02-4B4C-9493-A78D22C44988}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="276225" y="7343775"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1547,10 +1949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,10 +1976,10 @@
       <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="22"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1585,102 +1987,135 @@
         <v>4</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D3" s="7">
         <v>3</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="27"/>
+      <c r="F3" s="19"/>
     </row>
-    <row r="4" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D4" s="7">
         <v>5</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="24"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7">
+        <v>5</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="8">
-        <f>SUM(D3:D4)</f>
+      <c r="C6" s="23"/>
+      <c r="D6" s="8">
+        <f>SUM(D3:D5)</f>
+        <v>13</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:6" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:6" ht="346.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="25"/>
+      <c r="D10" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="15" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:6" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="11"/>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:6" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="15"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:6" ht="346.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="15" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="12" t="s">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="14"/>
+      <c r="C14" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="D14:E14"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>